<commit_message>
Second to last report commit
</commit_message>
<xml_diff>
--- a/Considerations.xlsx
+++ b/Considerations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lukas\Documents\MechProjELS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CEC9505-D7E9-4001-8BF3-87070835621D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD9E8C2-2051-44DE-BAE2-8E8388645D0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="753" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="5325" windowWidth="29040" windowHeight="15840" tabRatio="753" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Offene Fragen  Risiken" sheetId="9" r:id="rId1"/>
@@ -375,13 +375,7 @@
     <t>Vollständige Systemintegration</t>
   </si>
   <si>
-    <t>Done</t>
-  </si>
-  <si>
     <t>In work</t>
-  </si>
-  <si>
-    <t>Open</t>
   </si>
   <si>
     <t>Anforderung</t>
@@ -676,6 +670,12 @@
   </si>
   <si>
     <t>&gt; 10</t>
+  </si>
+  <si>
+    <t>Finished In time</t>
+  </si>
+  <si>
+    <t>Extra Time</t>
   </si>
 </sst>
 </file>
@@ -1316,7 +1316,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1457,9 +1457,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
@@ -1469,21 +1508,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1496,15 +1523,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1517,6 +1535,57 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1544,15 +1613,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1565,84 +1628,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
@@ -2013,52 +2021,52 @@
   <sheetData>
     <row r="7" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="37" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D7" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="F7" s="37" t="s">
+        <v>118</v>
+      </c>
+      <c r="G7" s="37" t="s">
+        <v>119</v>
+      </c>
+      <c r="H7" s="67" t="s">
+        <v>117</v>
+      </c>
+      <c r="I7" s="67"/>
+      <c r="J7" s="67"/>
+      <c r="K7" s="67"/>
+      <c r="L7" s="67"/>
+      <c r="M7" s="28" t="s">
         <v>114</v>
       </c>
-      <c r="E7" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="F7" s="37" t="s">
-        <v>120</v>
-      </c>
-      <c r="G7" s="37" t="s">
-        <v>121</v>
-      </c>
-      <c r="H7" s="56" t="s">
-        <v>119</v>
-      </c>
-      <c r="I7" s="56"/>
-      <c r="J7" s="56"/>
-      <c r="K7" s="56"/>
-      <c r="L7" s="56"/>
-      <c r="M7" s="28" t="s">
-        <v>116</v>
-      </c>
       <c r="N7" s="28" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G8" s="36"/>
-      <c r="H8" s="56"/>
-      <c r="I8" s="56"/>
-      <c r="J8" s="56"/>
-      <c r="K8" s="56"/>
-      <c r="L8" s="56"/>
+      <c r="H8" s="67"/>
+      <c r="I8" s="67"/>
+      <c r="J8" s="67"/>
+      <c r="K8" s="67"/>
+      <c r="L8" s="67"/>
       <c r="M8" s="33" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="N8" s="32" t="s">
         <v>3</v>
@@ -2066,25 +2074,25 @@
     </row>
     <row r="9" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D9" s="32" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E9" s="31" t="s">
         <v>59</v>
       </c>
       <c r="G9" s="36"/>
-      <c r="H9" s="56"/>
-      <c r="I9" s="56"/>
-      <c r="J9" s="56"/>
-      <c r="K9" s="56"/>
-      <c r="L9" s="56"/>
+      <c r="H9" s="67"/>
+      <c r="I9" s="67"/>
+      <c r="J9" s="67"/>
+      <c r="K9" s="67"/>
+      <c r="L9" s="67"/>
       <c r="M9" s="34" t="s">
         <v>59</v>
       </c>
       <c r="N9" s="32" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="3:14" ht="30" x14ac:dyDescent="0.25">
@@ -2092,19 +2100,19 @@
         <v>62</v>
       </c>
       <c r="D10" s="32" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E10" s="31" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G10" s="36"/>
-      <c r="H10" s="56"/>
-      <c r="I10" s="56"/>
-      <c r="J10" s="56"/>
-      <c r="K10" s="56"/>
-      <c r="L10" s="56"/>
+      <c r="H10" s="67"/>
+      <c r="I10" s="67"/>
+      <c r="J10" s="67"/>
+      <c r="K10" s="67"/>
+      <c r="L10" s="67"/>
       <c r="M10" s="35" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="N10" s="32" t="s">
         <v>4</v>
@@ -2115,19 +2123,19 @@
         <v>3</v>
       </c>
       <c r="D11" s="32" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E11" s="31" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G11" s="36"/>
-      <c r="H11" s="56"/>
-      <c r="I11" s="56"/>
-      <c r="J11" s="56"/>
-      <c r="K11" s="56"/>
-      <c r="L11" s="56"/>
+      <c r="H11" s="67"/>
+      <c r="I11" s="67"/>
+      <c r="J11" s="67"/>
+      <c r="K11" s="67"/>
+      <c r="L11" s="67"/>
       <c r="N11" s="32" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.25">
@@ -2135,103 +2143,103 @@
         <v>4</v>
       </c>
       <c r="D12" s="32" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E12" s="31" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G12" s="36"/>
-      <c r="H12" s="56"/>
-      <c r="I12" s="56"/>
-      <c r="J12" s="56"/>
-      <c r="K12" s="56"/>
-      <c r="L12" s="56"/>
+      <c r="H12" s="67"/>
+      <c r="I12" s="67"/>
+      <c r="J12" s="67"/>
+      <c r="K12" s="67"/>
+      <c r="L12" s="67"/>
       <c r="N12" s="32" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13" spans="3:14" x14ac:dyDescent="0.25">
       <c r="G13" s="36"/>
-      <c r="H13" s="56"/>
-      <c r="I13" s="56"/>
-      <c r="J13" s="56"/>
-      <c r="K13" s="56"/>
-      <c r="L13" s="56"/>
+      <c r="H13" s="67"/>
+      <c r="I13" s="67"/>
+      <c r="J13" s="67"/>
+      <c r="K13" s="67"/>
+      <c r="L13" s="67"/>
       <c r="N13" s="32" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="14" spans="3:14" x14ac:dyDescent="0.25">
       <c r="G14" s="36"/>
-      <c r="H14" s="56"/>
-      <c r="I14" s="56"/>
-      <c r="J14" s="56"/>
-      <c r="K14" s="56"/>
-      <c r="L14" s="56"/>
+      <c r="H14" s="67"/>
+      <c r="I14" s="67"/>
+      <c r="J14" s="67"/>
+      <c r="K14" s="67"/>
+      <c r="L14" s="67"/>
     </row>
     <row r="15" spans="3:14" x14ac:dyDescent="0.25">
       <c r="G15" s="36"/>
-      <c r="H15" s="56"/>
-      <c r="I15" s="56"/>
-      <c r="J15" s="56"/>
-      <c r="K15" s="56"/>
-      <c r="L15" s="56"/>
+      <c r="H15" s="67"/>
+      <c r="I15" s="67"/>
+      <c r="J15" s="67"/>
+      <c r="K15" s="67"/>
+      <c r="L15" s="67"/>
     </row>
     <row r="16" spans="3:14" x14ac:dyDescent="0.25">
       <c r="G16" s="36"/>
-      <c r="H16" s="56"/>
-      <c r="I16" s="56"/>
-      <c r="J16" s="56"/>
-      <c r="K16" s="56"/>
-      <c r="L16" s="56"/>
+      <c r="H16" s="67"/>
+      <c r="I16" s="67"/>
+      <c r="J16" s="67"/>
+      <c r="K16" s="67"/>
+      <c r="L16" s="67"/>
     </row>
     <row r="17" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G17" s="36"/>
-      <c r="H17" s="56"/>
-      <c r="I17" s="56"/>
-      <c r="J17" s="56"/>
-      <c r="K17" s="56"/>
-      <c r="L17" s="56"/>
+      <c r="H17" s="67"/>
+      <c r="I17" s="67"/>
+      <c r="J17" s="67"/>
+      <c r="K17" s="67"/>
+      <c r="L17" s="67"/>
     </row>
     <row r="18" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G18" s="36"/>
-      <c r="H18" s="56"/>
-      <c r="I18" s="56"/>
-      <c r="J18" s="56"/>
-      <c r="K18" s="56"/>
-      <c r="L18" s="56"/>
+      <c r="H18" s="67"/>
+      <c r="I18" s="67"/>
+      <c r="J18" s="67"/>
+      <c r="K18" s="67"/>
+      <c r="L18" s="67"/>
     </row>
     <row r="19" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G19" s="36"/>
-      <c r="H19" s="56"/>
-      <c r="I19" s="56"/>
-      <c r="J19" s="56"/>
-      <c r="K19" s="56"/>
-      <c r="L19" s="56"/>
+      <c r="H19" s="67"/>
+      <c r="I19" s="67"/>
+      <c r="J19" s="67"/>
+      <c r="K19" s="67"/>
+      <c r="L19" s="67"/>
     </row>
     <row r="20" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G20" s="36"/>
-      <c r="H20" s="56"/>
-      <c r="I20" s="56"/>
-      <c r="J20" s="56"/>
-      <c r="K20" s="56"/>
-      <c r="L20" s="56"/>
+      <c r="H20" s="67"/>
+      <c r="I20" s="67"/>
+      <c r="J20" s="67"/>
+      <c r="K20" s="67"/>
+      <c r="L20" s="67"/>
     </row>
     <row r="21" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G21" s="36"/>
-      <c r="H21" s="56"/>
-      <c r="I21" s="56"/>
-      <c r="J21" s="56"/>
-      <c r="K21" s="56"/>
-      <c r="L21" s="56"/>
+      <c r="H21" s="67"/>
+      <c r="I21" s="67"/>
+      <c r="J21" s="67"/>
+      <c r="K21" s="67"/>
+      <c r="L21" s="67"/>
     </row>
     <row r="22" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G22" s="36"/>
-      <c r="H22" s="56"/>
-      <c r="I22" s="56"/>
-      <c r="J22" s="56"/>
-      <c r="K22" s="56"/>
-      <c r="L22" s="56"/>
+      <c r="H22" s="67"/>
+      <c r="I22" s="67"/>
+      <c r="J22" s="67"/>
+      <c r="K22" s="67"/>
+      <c r="L22" s="67"/>
     </row>
     <row r="23" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G23" s="36"/>
@@ -2311,12 +2319,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD42D481-3DE8-4CF1-900C-17766BD9A35E}">
   <dimension ref="A2:BS27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="BZ31" sqref="BZ31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="BZ14" sqref="BZ14:CC25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="72" width="1.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2333,282 +2342,282 @@
     <row r="3" spans="1:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
-        <v>97</v>
+        <v>192</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C4" s="62" t="s">
+      <c r="C4" s="68" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="62"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
-      <c r="H4" s="62"/>
-      <c r="I4" s="62"/>
-      <c r="J4" s="62"/>
-      <c r="K4" s="62" t="s">
+      <c r="D4" s="68"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="68"/>
+      <c r="I4" s="68"/>
+      <c r="J4" s="68"/>
+      <c r="K4" s="68" t="s">
         <v>70</v>
       </c>
-      <c r="L4" s="62"/>
-      <c r="M4" s="62"/>
-      <c r="N4" s="62"/>
-      <c r="O4" s="62"/>
-      <c r="P4" s="62"/>
-      <c r="Q4" s="62"/>
-      <c r="R4" s="62"/>
-      <c r="S4" s="62" t="s">
+      <c r="L4" s="68"/>
+      <c r="M4" s="68"/>
+      <c r="N4" s="68"/>
+      <c r="O4" s="68"/>
+      <c r="P4" s="68"/>
+      <c r="Q4" s="68"/>
+      <c r="R4" s="68"/>
+      <c r="S4" s="68" t="s">
         <v>71</v>
       </c>
-      <c r="T4" s="62"/>
-      <c r="U4" s="62"/>
-      <c r="V4" s="62"/>
-      <c r="W4" s="62"/>
-      <c r="X4" s="62"/>
-      <c r="Y4" s="62"/>
-      <c r="Z4" s="62"/>
-      <c r="AA4" s="62" t="s">
+      <c r="T4" s="68"/>
+      <c r="U4" s="68"/>
+      <c r="V4" s="68"/>
+      <c r="W4" s="68"/>
+      <c r="X4" s="68"/>
+      <c r="Y4" s="68"/>
+      <c r="Z4" s="68"/>
+      <c r="AA4" s="68" t="s">
         <v>72</v>
       </c>
-      <c r="AB4" s="62"/>
-      <c r="AC4" s="62"/>
-      <c r="AD4" s="62"/>
-      <c r="AE4" s="62"/>
-      <c r="AF4" s="62" t="s">
+      <c r="AB4" s="68"/>
+      <c r="AC4" s="68"/>
+      <c r="AD4" s="68"/>
+      <c r="AE4" s="68"/>
+      <c r="AF4" s="68" t="s">
         <v>73</v>
       </c>
-      <c r="AG4" s="62"/>
-      <c r="AH4" s="62"/>
-      <c r="AI4" s="62"/>
-      <c r="AJ4" s="62"/>
-      <c r="AK4" s="62" t="s">
+      <c r="AG4" s="68"/>
+      <c r="AH4" s="68"/>
+      <c r="AI4" s="68"/>
+      <c r="AJ4" s="68"/>
+      <c r="AK4" s="68" t="s">
         <v>74</v>
       </c>
-      <c r="AL4" s="62"/>
-      <c r="AM4" s="62"/>
-      <c r="AN4" s="62"/>
-      <c r="AO4" s="62"/>
-      <c r="AP4" s="62" t="s">
+      <c r="AL4" s="68"/>
+      <c r="AM4" s="68"/>
+      <c r="AN4" s="68"/>
+      <c r="AO4" s="68"/>
+      <c r="AP4" s="68" t="s">
         <v>75</v>
       </c>
-      <c r="AQ4" s="62"/>
-      <c r="AR4" s="62"/>
-      <c r="AS4" s="62"/>
-      <c r="AT4" s="62"/>
-      <c r="AU4" s="62" t="s">
+      <c r="AQ4" s="68"/>
+      <c r="AR4" s="68"/>
+      <c r="AS4" s="68"/>
+      <c r="AT4" s="68"/>
+      <c r="AU4" s="68" t="s">
         <v>76</v>
       </c>
-      <c r="AV4" s="62"/>
-      <c r="AW4" s="62"/>
-      <c r="AX4" s="62"/>
-      <c r="AY4" s="62"/>
-      <c r="AZ4" s="62" t="s">
+      <c r="AV4" s="68"/>
+      <c r="AW4" s="68"/>
+      <c r="AX4" s="68"/>
+      <c r="AY4" s="68"/>
+      <c r="AZ4" s="68" t="s">
         <v>67</v>
       </c>
-      <c r="BA4" s="62"/>
-      <c r="BB4" s="62"/>
-      <c r="BC4" s="62"/>
-      <c r="BD4" s="62"/>
-      <c r="BE4" s="62"/>
-      <c r="BF4" s="62"/>
-      <c r="BG4" s="62"/>
-      <c r="BH4" s="62"/>
-      <c r="BI4" s="62"/>
-      <c r="BJ4" s="62" t="s">
+      <c r="BA4" s="68"/>
+      <c r="BB4" s="68"/>
+      <c r="BC4" s="68"/>
+      <c r="BD4" s="68"/>
+      <c r="BE4" s="68"/>
+      <c r="BF4" s="68"/>
+      <c r="BG4" s="68"/>
+      <c r="BH4" s="68"/>
+      <c r="BI4" s="68"/>
+      <c r="BJ4" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="BK4" s="62"/>
-      <c r="BL4" s="62"/>
-      <c r="BM4" s="62"/>
-      <c r="BN4" s="62"/>
-      <c r="BO4" s="62"/>
-      <c r="BP4" s="62"/>
-      <c r="BQ4" s="62"/>
-      <c r="BR4" s="62"/>
-      <c r="BS4" s="63"/>
+      <c r="BK4" s="68"/>
+      <c r="BL4" s="68"/>
+      <c r="BM4" s="68"/>
+      <c r="BN4" s="68"/>
+      <c r="BO4" s="68"/>
+      <c r="BP4" s="68"/>
+      <c r="BQ4" s="68"/>
+      <c r="BR4" s="68"/>
+      <c r="BS4" s="73"/>
     </row>
     <row r="5" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A5" s="28"/>
       <c r="B5" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="66" t="s">
+      <c r="C5" s="75" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="66"/>
-      <c r="I5" s="66"/>
-      <c r="J5" s="66"/>
-      <c r="K5" s="66"/>
-      <c r="L5" s="66"/>
-      <c r="M5" s="66"/>
-      <c r="N5" s="66"/>
-      <c r="O5" s="66"/>
-      <c r="P5" s="66"/>
-      <c r="Q5" s="66"/>
-      <c r="R5" s="66"/>
-      <c r="S5" s="66"/>
-      <c r="T5" s="66"/>
-      <c r="U5" s="66"/>
-      <c r="V5" s="66"/>
-      <c r="W5" s="66"/>
-      <c r="X5" s="66"/>
-      <c r="Y5" s="66"/>
-      <c r="Z5" s="66"/>
-      <c r="AA5" s="66" t="s">
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="75"/>
+      <c r="I5" s="75"/>
+      <c r="J5" s="75"/>
+      <c r="K5" s="75"/>
+      <c r="L5" s="75"/>
+      <c r="M5" s="75"/>
+      <c r="N5" s="75"/>
+      <c r="O5" s="75"/>
+      <c r="P5" s="75"/>
+      <c r="Q5" s="75"/>
+      <c r="R5" s="75"/>
+      <c r="S5" s="75"/>
+      <c r="T5" s="75"/>
+      <c r="U5" s="75"/>
+      <c r="V5" s="75"/>
+      <c r="W5" s="75"/>
+      <c r="X5" s="75"/>
+      <c r="Y5" s="75"/>
+      <c r="Z5" s="75"/>
+      <c r="AA5" s="75" t="s">
         <v>78</v>
       </c>
-      <c r="AB5" s="66"/>
-      <c r="AC5" s="66"/>
-      <c r="AD5" s="66"/>
-      <c r="AE5" s="66"/>
-      <c r="AF5" s="66"/>
-      <c r="AG5" s="66"/>
-      <c r="AH5" s="66"/>
-      <c r="AI5" s="66"/>
-      <c r="AJ5" s="66"/>
-      <c r="AK5" s="66"/>
-      <c r="AL5" s="66"/>
-      <c r="AM5" s="66"/>
-      <c r="AN5" s="66"/>
-      <c r="AO5" s="66"/>
-      <c r="AP5" s="66"/>
-      <c r="AQ5" s="66"/>
-      <c r="AR5" s="66"/>
-      <c r="AS5" s="66"/>
-      <c r="AT5" s="66"/>
-      <c r="AU5" s="66"/>
-      <c r="AV5" s="66"/>
-      <c r="AW5" s="66"/>
-      <c r="AX5" s="66"/>
-      <c r="AY5" s="66"/>
-      <c r="AZ5" s="66"/>
-      <c r="BA5" s="66"/>
-      <c r="BB5" s="66"/>
-      <c r="BC5" s="66"/>
-      <c r="BD5" s="66"/>
-      <c r="BE5" s="66"/>
-      <c r="BF5" s="66"/>
-      <c r="BG5" s="66"/>
-      <c r="BH5" s="66"/>
-      <c r="BI5" s="66"/>
-      <c r="BJ5" s="66"/>
-      <c r="BK5" s="66"/>
-      <c r="BL5" s="66"/>
-      <c r="BM5" s="66"/>
-      <c r="BN5" s="66"/>
-      <c r="BO5" s="66"/>
-      <c r="BP5" s="66"/>
-      <c r="BQ5" s="66"/>
-      <c r="BR5" s="66"/>
-      <c r="BS5" s="67"/>
+      <c r="AB5" s="75"/>
+      <c r="AC5" s="75"/>
+      <c r="AD5" s="75"/>
+      <c r="AE5" s="75"/>
+      <c r="AF5" s="75"/>
+      <c r="AG5" s="75"/>
+      <c r="AH5" s="75"/>
+      <c r="AI5" s="75"/>
+      <c r="AJ5" s="75"/>
+      <c r="AK5" s="75"/>
+      <c r="AL5" s="75"/>
+      <c r="AM5" s="75"/>
+      <c r="AN5" s="75"/>
+      <c r="AO5" s="75"/>
+      <c r="AP5" s="75"/>
+      <c r="AQ5" s="75"/>
+      <c r="AR5" s="75"/>
+      <c r="AS5" s="75"/>
+      <c r="AT5" s="75"/>
+      <c r="AU5" s="75"/>
+      <c r="AV5" s="75"/>
+      <c r="AW5" s="75"/>
+      <c r="AX5" s="75"/>
+      <c r="AY5" s="75"/>
+      <c r="AZ5" s="75"/>
+      <c r="BA5" s="75"/>
+      <c r="BB5" s="75"/>
+      <c r="BC5" s="75"/>
+      <c r="BD5" s="75"/>
+      <c r="BE5" s="75"/>
+      <c r="BF5" s="75"/>
+      <c r="BG5" s="75"/>
+      <c r="BH5" s="75"/>
+      <c r="BI5" s="75"/>
+      <c r="BJ5" s="75"/>
+      <c r="BK5" s="75"/>
+      <c r="BL5" s="75"/>
+      <c r="BM5" s="75"/>
+      <c r="BN5" s="75"/>
+      <c r="BO5" s="75"/>
+      <c r="BP5" s="75"/>
+      <c r="BQ5" s="75"/>
+      <c r="BR5" s="75"/>
+      <c r="BS5" s="76"/>
     </row>
     <row r="6" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="68" t="s">
+      <c r="C6" s="77" t="s">
         <v>81</v>
       </c>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="68"/>
-      <c r="G6" s="68"/>
-      <c r="H6" s="68"/>
-      <c r="I6" s="68"/>
-      <c r="J6" s="68"/>
-      <c r="K6" s="68"/>
-      <c r="L6" s="68"/>
-      <c r="M6" s="68"/>
-      <c r="N6" s="68"/>
-      <c r="O6" s="68"/>
-      <c r="P6" s="68"/>
-      <c r="Q6" s="68"/>
-      <c r="R6" s="68"/>
-      <c r="S6" s="68"/>
-      <c r="T6" s="68"/>
-      <c r="U6" s="68"/>
-      <c r="V6" s="68"/>
-      <c r="W6" s="68"/>
-      <c r="X6" s="68"/>
-      <c r="Y6" s="68"/>
-      <c r="Z6" s="68"/>
-      <c r="AA6" s="64" t="s">
+      <c r="D6" s="77"/>
+      <c r="E6" s="77"/>
+      <c r="F6" s="77"/>
+      <c r="G6" s="77"/>
+      <c r="H6" s="77"/>
+      <c r="I6" s="77"/>
+      <c r="J6" s="77"/>
+      <c r="K6" s="77"/>
+      <c r="L6" s="77"/>
+      <c r="M6" s="77"/>
+      <c r="N6" s="77"/>
+      <c r="O6" s="77"/>
+      <c r="P6" s="77"/>
+      <c r="Q6" s="77"/>
+      <c r="R6" s="77"/>
+      <c r="S6" s="77"/>
+      <c r="T6" s="77"/>
+      <c r="U6" s="77"/>
+      <c r="V6" s="77"/>
+      <c r="W6" s="77"/>
+      <c r="X6" s="77"/>
+      <c r="Y6" s="77"/>
+      <c r="Z6" s="77"/>
+      <c r="AA6" s="69" t="s">
         <v>82</v>
       </c>
-      <c r="AB6" s="64"/>
-      <c r="AC6" s="64"/>
-      <c r="AD6" s="64"/>
-      <c r="AE6" s="64"/>
-      <c r="AF6" s="64"/>
-      <c r="AG6" s="64"/>
-      <c r="AH6" s="64"/>
-      <c r="AI6" s="64"/>
-      <c r="AJ6" s="64"/>
-      <c r="AK6" s="64"/>
-      <c r="AL6" s="64"/>
-      <c r="AM6" s="64"/>
-      <c r="AN6" s="64"/>
-      <c r="AO6" s="64"/>
-      <c r="AP6" s="64"/>
-      <c r="AQ6" s="64"/>
-      <c r="AR6" s="64"/>
-      <c r="AS6" s="64"/>
-      <c r="AT6" s="64"/>
-      <c r="AU6" s="64"/>
-      <c r="AV6" s="64"/>
-      <c r="AW6" s="64"/>
-      <c r="AX6" s="64"/>
-      <c r="AY6" s="64"/>
-      <c r="AZ6" s="64" t="s">
+      <c r="AB6" s="69"/>
+      <c r="AC6" s="69"/>
+      <c r="AD6" s="69"/>
+      <c r="AE6" s="69"/>
+      <c r="AF6" s="69"/>
+      <c r="AG6" s="69"/>
+      <c r="AH6" s="69"/>
+      <c r="AI6" s="69"/>
+      <c r="AJ6" s="69"/>
+      <c r="AK6" s="69"/>
+      <c r="AL6" s="69"/>
+      <c r="AM6" s="69"/>
+      <c r="AN6" s="69"/>
+      <c r="AO6" s="69"/>
+      <c r="AP6" s="69"/>
+      <c r="AQ6" s="69"/>
+      <c r="AR6" s="69"/>
+      <c r="AS6" s="69"/>
+      <c r="AT6" s="69"/>
+      <c r="AU6" s="69"/>
+      <c r="AV6" s="69"/>
+      <c r="AW6" s="69"/>
+      <c r="AX6" s="69"/>
+      <c r="AY6" s="69"/>
+      <c r="AZ6" s="69" t="s">
         <v>83</v>
       </c>
-      <c r="BA6" s="64"/>
-      <c r="BB6" s="64"/>
-      <c r="BC6" s="64"/>
-      <c r="BD6" s="64"/>
-      <c r="BE6" s="64"/>
-      <c r="BF6" s="64"/>
-      <c r="BG6" s="64"/>
-      <c r="BH6" s="64"/>
-      <c r="BI6" s="64"/>
-      <c r="BJ6" s="64"/>
-      <c r="BK6" s="64"/>
-      <c r="BL6" s="64"/>
-      <c r="BM6" s="64"/>
-      <c r="BN6" s="64"/>
-      <c r="BO6" s="64"/>
-      <c r="BP6" s="64"/>
-      <c r="BQ6" s="64"/>
-      <c r="BR6" s="64"/>
-      <c r="BS6" s="65"/>
+      <c r="BA6" s="69"/>
+      <c r="BB6" s="69"/>
+      <c r="BC6" s="69"/>
+      <c r="BD6" s="69"/>
+      <c r="BE6" s="69"/>
+      <c r="BF6" s="69"/>
+      <c r="BG6" s="69"/>
+      <c r="BH6" s="69"/>
+      <c r="BI6" s="69"/>
+      <c r="BJ6" s="69"/>
+      <c r="BK6" s="69"/>
+      <c r="BL6" s="69"/>
+      <c r="BM6" s="69"/>
+      <c r="BN6" s="69"/>
+      <c r="BO6" s="69"/>
+      <c r="BP6" s="69"/>
+      <c r="BQ6" s="69"/>
+      <c r="BR6" s="69"/>
+      <c r="BS6" s="74"/>
     </row>
     <row r="7" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A7" s="28"/>
-      <c r="B7" s="57" t="s">
+      <c r="B7" s="70" t="s">
         <v>84</v>
       </c>
-      <c r="C7" s="60" t="s">
+      <c r="C7" s="113" t="s">
         <v>90</v>
       </c>
-      <c r="D7" s="60"/>
-      <c r="E7" s="60"/>
-      <c r="F7" s="60"/>
-      <c r="G7" s="60"/>
-      <c r="H7" s="60"/>
-      <c r="I7" s="60"/>
-      <c r="J7" s="60"/>
-      <c r="K7" s="60"/>
-      <c r="L7" s="60"/>
-      <c r="M7" s="60"/>
-      <c r="N7" s="60"/>
+      <c r="D7" s="113"/>
+      <c r="E7" s="113"/>
+      <c r="F7" s="113"/>
+      <c r="G7" s="113"/>
+      <c r="H7" s="113"/>
+      <c r="I7" s="113"/>
+      <c r="J7" s="113"/>
+      <c r="K7" s="113"/>
+      <c r="L7" s="113"/>
+      <c r="M7" s="113"/>
+      <c r="N7" s="113"/>
       <c r="O7" s="23"/>
       <c r="P7" s="23"/>
       <c r="Q7" s="23"/>
@@ -2669,9 +2678,9 @@
     </row>
     <row r="8" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A8" s="30" t="s">
-        <v>99</v>
-      </c>
-      <c r="B8" s="58"/>
+        <v>193</v>
+      </c>
+      <c r="B8" s="71"/>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
@@ -2724,22 +2733,22 @@
       <c r="BS8" s="6"/>
     </row>
     <row r="9" spans="1:71" x14ac:dyDescent="0.25">
-      <c r="B9" s="58"/>
+      <c r="B9" s="71"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
-      <c r="F9" s="61" t="s">
+      <c r="F9" s="114" t="s">
         <v>85</v>
       </c>
-      <c r="G9" s="61"/>
-      <c r="H9" s="61"/>
-      <c r="I9" s="61"/>
-      <c r="J9" s="61"/>
-      <c r="K9" s="61"/>
-      <c r="L9" s="61"/>
-      <c r="M9" s="61"/>
-      <c r="N9" s="61"/>
-      <c r="O9" s="61"/>
+      <c r="G9" s="114"/>
+      <c r="H9" s="114"/>
+      <c r="I9" s="114"/>
+      <c r="J9" s="114"/>
+      <c r="K9" s="114"/>
+      <c r="L9" s="114"/>
+      <c r="M9" s="114"/>
+      <c r="N9" s="114"/>
+      <c r="O9" s="114"/>
       <c r="P9" s="13"/>
       <c r="Q9" s="13"/>
       <c r="R9" s="13"/>
@@ -2798,7 +2807,7 @@
       <c r="BS9" s="6"/>
     </row>
     <row r="10" spans="1:71" x14ac:dyDescent="0.25">
-      <c r="B10" s="58"/>
+      <c r="B10" s="71"/>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
@@ -2850,34 +2859,34 @@
       <c r="BS10" s="6"/>
     </row>
     <row r="11" spans="1:71" x14ac:dyDescent="0.25">
-      <c r="B11" s="58"/>
+      <c r="B11" s="71"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
-      <c r="F11" s="61" t="s">
+      <c r="F11" s="114" t="s">
         <v>86</v>
       </c>
-      <c r="G11" s="61"/>
-      <c r="H11" s="61"/>
-      <c r="I11" s="61"/>
-      <c r="J11" s="61"/>
-      <c r="K11" s="61"/>
-      <c r="L11" s="61"/>
-      <c r="M11" s="61"/>
-      <c r="N11" s="61"/>
-      <c r="O11" s="61"/>
-      <c r="P11" s="61"/>
-      <c r="Q11" s="61"/>
-      <c r="R11" s="61"/>
-      <c r="S11" s="61"/>
-      <c r="T11" s="13"/>
-      <c r="U11" s="13"/>
-      <c r="V11" s="13"/>
-      <c r="W11" s="13"/>
-      <c r="X11" s="13"/>
-      <c r="Y11" s="13"/>
-      <c r="Z11" s="18"/>
-      <c r="AA11" s="19"/>
+      <c r="G11" s="114"/>
+      <c r="H11" s="114"/>
+      <c r="I11" s="114"/>
+      <c r="J11" s="114"/>
+      <c r="K11" s="114"/>
+      <c r="L11" s="114"/>
+      <c r="M11" s="114"/>
+      <c r="N11" s="114"/>
+      <c r="O11" s="114"/>
+      <c r="P11" s="114"/>
+      <c r="Q11" s="114"/>
+      <c r="R11" s="114"/>
+      <c r="S11" s="114"/>
+      <c r="T11" s="118"/>
+      <c r="U11" s="118"/>
+      <c r="V11" s="118"/>
+      <c r="W11" s="118"/>
+      <c r="X11" s="118"/>
+      <c r="Y11" s="118"/>
+      <c r="Z11" s="117"/>
+      <c r="AA11" s="119"/>
       <c r="AB11" s="13"/>
       <c r="AC11" s="13"/>
       <c r="AD11" s="13"/>
@@ -2924,7 +2933,7 @@
       <c r="BS11" s="6"/>
     </row>
     <row r="12" spans="1:71" x14ac:dyDescent="0.25">
-      <c r="B12" s="58"/>
+      <c r="B12" s="71"/>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
@@ -2980,67 +2989,67 @@
       <c r="BS12" s="6"/>
     </row>
     <row r="13" spans="1:71" x14ac:dyDescent="0.25">
-      <c r="B13" s="58"/>
+      <c r="B13" s="71"/>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
-      <c r="I13" s="69" t="s">
+      <c r="I13" s="114" t="s">
         <v>87</v>
       </c>
-      <c r="J13" s="69"/>
-      <c r="K13" s="69"/>
-      <c r="L13" s="69"/>
-      <c r="M13" s="69"/>
-      <c r="N13" s="69"/>
-      <c r="O13" s="69"/>
-      <c r="P13" s="69"/>
-      <c r="Q13" s="69"/>
-      <c r="R13" s="69"/>
-      <c r="S13" s="69"/>
-      <c r="T13" s="69"/>
-      <c r="U13" s="69"/>
-      <c r="V13" s="69"/>
-      <c r="W13" s="69"/>
-      <c r="X13" s="13"/>
-      <c r="Y13" s="13"/>
-      <c r="Z13" s="18"/>
-      <c r="AA13" s="19"/>
-      <c r="AB13" s="13"/>
-      <c r="AC13" s="13"/>
-      <c r="AD13" s="13"/>
-      <c r="AE13" s="13"/>
-      <c r="AF13" s="13"/>
-      <c r="AG13" s="13"/>
-      <c r="AH13" s="13"/>
-      <c r="AI13" s="12"/>
-      <c r="AJ13" s="12"/>
-      <c r="AK13" s="12"/>
-      <c r="AL13" s="12"/>
-      <c r="AM13" s="12"/>
-      <c r="AN13" s="12"/>
-      <c r="AO13" s="12"/>
-      <c r="AP13" s="12"/>
-      <c r="AQ13" s="12"/>
-      <c r="AR13" s="12"/>
-      <c r="AS13" s="12"/>
-      <c r="AT13" s="12"/>
-      <c r="AU13" s="12"/>
-      <c r="AV13" s="12"/>
-      <c r="AW13" s="12"/>
-      <c r="AX13" s="12"/>
-      <c r="AY13" s="25"/>
-      <c r="AZ13" s="12"/>
-      <c r="BA13" s="12"/>
-      <c r="BB13" s="12"/>
-      <c r="BC13" s="12"/>
-      <c r="BD13" s="12"/>
-      <c r="BE13" s="12"/>
-      <c r="BF13" s="12"/>
-      <c r="BG13" s="12"/>
-      <c r="BH13" s="12"/>
+      <c r="J13" s="114"/>
+      <c r="K13" s="114"/>
+      <c r="L13" s="114"/>
+      <c r="M13" s="114"/>
+      <c r="N13" s="114"/>
+      <c r="O13" s="114"/>
+      <c r="P13" s="114"/>
+      <c r="Q13" s="114"/>
+      <c r="R13" s="114"/>
+      <c r="S13" s="114"/>
+      <c r="T13" s="114"/>
+      <c r="U13" s="114"/>
+      <c r="V13" s="114"/>
+      <c r="W13" s="114"/>
+      <c r="X13" s="118"/>
+      <c r="Y13" s="118"/>
+      <c r="Z13" s="117"/>
+      <c r="AA13" s="119"/>
+      <c r="AB13" s="118"/>
+      <c r="AC13" s="118"/>
+      <c r="AD13" s="118"/>
+      <c r="AE13" s="118"/>
+      <c r="AF13" s="118"/>
+      <c r="AG13" s="118"/>
+      <c r="AH13" s="118"/>
+      <c r="AI13" s="120"/>
+      <c r="AJ13" s="120"/>
+      <c r="AK13" s="120"/>
+      <c r="AL13" s="120"/>
+      <c r="AM13" s="120"/>
+      <c r="AN13" s="120"/>
+      <c r="AO13" s="120"/>
+      <c r="AP13" s="120"/>
+      <c r="AQ13" s="120"/>
+      <c r="AR13" s="120"/>
+      <c r="AS13" s="120"/>
+      <c r="AT13" s="120"/>
+      <c r="AU13" s="120"/>
+      <c r="AV13" s="120"/>
+      <c r="AW13" s="120"/>
+      <c r="AX13" s="120"/>
+      <c r="AY13" s="121"/>
+      <c r="AZ13" s="120"/>
+      <c r="BA13" s="120"/>
+      <c r="BB13" s="120"/>
+      <c r="BC13" s="120"/>
+      <c r="BD13" s="120"/>
+      <c r="BE13" s="120"/>
+      <c r="BF13" s="120"/>
+      <c r="BG13" s="120"/>
+      <c r="BH13" s="120"/>
       <c r="BI13" s="12"/>
       <c r="BJ13" s="12"/>
       <c r="BK13" s="12"/>
@@ -3054,7 +3063,7 @@
       <c r="BS13" s="6"/>
     </row>
     <row r="14" spans="1:71" x14ac:dyDescent="0.25">
-      <c r="B14" s="58"/>
+      <c r="B14" s="71"/>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
@@ -3111,7 +3120,7 @@
       <c r="BS14" s="6"/>
     </row>
     <row r="15" spans="1:71" x14ac:dyDescent="0.25">
-      <c r="B15" s="58"/>
+      <c r="B15" s="71"/>
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
       <c r="E15" s="13"/>
@@ -3119,20 +3128,20 @@
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
       <c r="I15" s="13"/>
-      <c r="J15" s="69" t="s">
+      <c r="J15" s="114" t="s">
         <v>91</v>
       </c>
-      <c r="K15" s="69"/>
-      <c r="L15" s="69"/>
-      <c r="M15" s="69"/>
-      <c r="N15" s="69"/>
-      <c r="O15" s="69"/>
-      <c r="P15" s="69"/>
-      <c r="Q15" s="69"/>
-      <c r="R15" s="69"/>
-      <c r="S15" s="69"/>
-      <c r="T15" s="69"/>
-      <c r="U15" s="69"/>
+      <c r="K15" s="114"/>
+      <c r="L15" s="114"/>
+      <c r="M15" s="114"/>
+      <c r="N15" s="114"/>
+      <c r="O15" s="114"/>
+      <c r="P15" s="114"/>
+      <c r="Q15" s="114"/>
+      <c r="R15" s="114"/>
+      <c r="S15" s="114"/>
+      <c r="T15" s="114"/>
+      <c r="U15" s="114"/>
       <c r="V15" s="13"/>
       <c r="W15" s="13"/>
       <c r="X15" s="13"/>
@@ -3161,7 +3170,7 @@
       <c r="BS15" s="6"/>
     </row>
     <row r="16" spans="1:71" x14ac:dyDescent="0.25">
-      <c r="B16" s="58"/>
+      <c r="B16" s="71"/>
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
       <c r="E16" s="13"/>
@@ -3195,7 +3204,7 @@
       <c r="BS16" s="6"/>
     </row>
     <row r="17" spans="2:71" x14ac:dyDescent="0.25">
-      <c r="B17" s="58"/>
+      <c r="B17" s="71"/>
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>
       <c r="E17" s="13"/>
@@ -3204,40 +3213,40 @@
       <c r="H17" s="13"/>
       <c r="I17" s="13"/>
       <c r="J17" s="12"/>
-      <c r="K17" s="69" t="s">
+      <c r="K17" s="114" t="s">
         <v>88</v>
       </c>
-      <c r="L17" s="69"/>
-      <c r="M17" s="69"/>
-      <c r="N17" s="69"/>
-      <c r="O17" s="69"/>
-      <c r="P17" s="69"/>
-      <c r="Q17" s="69"/>
-      <c r="R17" s="69"/>
-      <c r="S17" s="69"/>
-      <c r="T17" s="69"/>
-      <c r="U17" s="69"/>
-      <c r="V17" s="69"/>
-      <c r="W17" s="69"/>
-      <c r="X17" s="13"/>
-      <c r="Y17" s="13"/>
-      <c r="Z17" s="18"/>
-      <c r="AA17" s="19"/>
-      <c r="AB17" s="13"/>
-      <c r="AC17" s="13"/>
-      <c r="AD17" s="13"/>
-      <c r="AE17" s="13"/>
-      <c r="AF17" s="13"/>
-      <c r="AG17" s="13"/>
-      <c r="AH17" s="13"/>
-      <c r="AI17" s="12"/>
-      <c r="AJ17" s="12"/>
-      <c r="AK17" s="12"/>
-      <c r="AL17" s="12"/>
-      <c r="AM17" s="12"/>
-      <c r="AN17" s="12"/>
-      <c r="AO17" s="12"/>
-      <c r="AP17" s="12"/>
+      <c r="L17" s="114"/>
+      <c r="M17" s="114"/>
+      <c r="N17" s="114"/>
+      <c r="O17" s="114"/>
+      <c r="P17" s="114"/>
+      <c r="Q17" s="114"/>
+      <c r="R17" s="114"/>
+      <c r="S17" s="114"/>
+      <c r="T17" s="114"/>
+      <c r="U17" s="114"/>
+      <c r="V17" s="114"/>
+      <c r="W17" s="114"/>
+      <c r="X17" s="118"/>
+      <c r="Y17" s="118"/>
+      <c r="Z17" s="117"/>
+      <c r="AA17" s="119"/>
+      <c r="AB17" s="118"/>
+      <c r="AC17" s="118"/>
+      <c r="AD17" s="118"/>
+      <c r="AE17" s="118"/>
+      <c r="AF17" s="118"/>
+      <c r="AG17" s="118"/>
+      <c r="AH17" s="118"/>
+      <c r="AI17" s="120"/>
+      <c r="AJ17" s="120"/>
+      <c r="AK17" s="120"/>
+      <c r="AL17" s="120"/>
+      <c r="AM17" s="120"/>
+      <c r="AN17" s="120"/>
+      <c r="AO17" s="120"/>
+      <c r="AP17" s="120"/>
       <c r="AQ17" s="12"/>
       <c r="AR17" s="12"/>
       <c r="AS17" s="12"/>
@@ -3268,7 +3277,7 @@
       <c r="BS17" s="6"/>
     </row>
     <row r="18" spans="2:71" x14ac:dyDescent="0.25">
-      <c r="B18" s="58"/>
+      <c r="B18" s="71"/>
       <c r="C18" s="13"/>
       <c r="D18" s="13"/>
       <c r="E18" s="13"/>
@@ -3325,7 +3334,7 @@
       <c r="BS18" s="6"/>
     </row>
     <row r="19" spans="2:71" x14ac:dyDescent="0.25">
-      <c r="B19" s="58"/>
+      <c r="B19" s="71"/>
       <c r="C19" s="13"/>
       <c r="D19" s="13"/>
       <c r="E19" s="13"/>
@@ -3334,22 +3343,22 @@
       <c r="H19" s="13"/>
       <c r="I19" s="13"/>
       <c r="J19" s="13"/>
-      <c r="K19" s="69" t="s">
+      <c r="K19" s="114" t="s">
         <v>89</v>
       </c>
-      <c r="L19" s="69"/>
-      <c r="M19" s="69"/>
-      <c r="N19" s="69"/>
-      <c r="O19" s="69"/>
-      <c r="P19" s="69"/>
-      <c r="Q19" s="69"/>
-      <c r="R19" s="69"/>
-      <c r="S19" s="69"/>
-      <c r="T19" s="69"/>
-      <c r="U19" s="69"/>
-      <c r="V19" s="69"/>
-      <c r="W19" s="69"/>
-      <c r="X19" s="69"/>
+      <c r="L19" s="114"/>
+      <c r="M19" s="114"/>
+      <c r="N19" s="114"/>
+      <c r="O19" s="114"/>
+      <c r="P19" s="114"/>
+      <c r="Q19" s="114"/>
+      <c r="R19" s="114"/>
+      <c r="S19" s="114"/>
+      <c r="T19" s="114"/>
+      <c r="U19" s="114"/>
+      <c r="V19" s="114"/>
+      <c r="W19" s="114"/>
+      <c r="X19" s="114"/>
       <c r="Y19" s="13"/>
       <c r="Z19" s="18"/>
       <c r="AA19" s="19"/>
@@ -3399,7 +3408,7 @@
       <c r="BS19" s="6"/>
     </row>
     <row r="20" spans="2:71" x14ac:dyDescent="0.25">
-      <c r="B20" s="58"/>
+      <c r="B20" s="71"/>
       <c r="C20" s="13"/>
       <c r="D20" s="13"/>
       <c r="E20" s="13"/>
@@ -3457,7 +3466,7 @@
       <c r="BS20" s="6"/>
     </row>
     <row r="21" spans="2:71" x14ac:dyDescent="0.25">
-      <c r="B21" s="58"/>
+      <c r="B21" s="71"/>
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
       <c r="E21" s="13"/>
@@ -3466,23 +3475,23 @@
       <c r="H21" s="13"/>
       <c r="I21" s="13"/>
       <c r="J21" s="13"/>
-      <c r="K21" s="69" t="s">
+      <c r="K21" s="114" t="s">
         <v>92</v>
       </c>
-      <c r="L21" s="69"/>
-      <c r="M21" s="69"/>
-      <c r="N21" s="69"/>
-      <c r="O21" s="69"/>
-      <c r="P21" s="69"/>
-      <c r="Q21" s="69"/>
-      <c r="R21" s="69"/>
-      <c r="S21" s="69"/>
-      <c r="T21" s="69"/>
-      <c r="U21" s="69"/>
-      <c r="V21" s="69"/>
-      <c r="W21" s="69"/>
-      <c r="X21" s="69"/>
-      <c r="Y21" s="69"/>
+      <c r="L21" s="114"/>
+      <c r="M21" s="114"/>
+      <c r="N21" s="114"/>
+      <c r="O21" s="114"/>
+      <c r="P21" s="114"/>
+      <c r="Q21" s="114"/>
+      <c r="R21" s="114"/>
+      <c r="S21" s="114"/>
+      <c r="T21" s="114"/>
+      <c r="U21" s="114"/>
+      <c r="V21" s="114"/>
+      <c r="W21" s="114"/>
+      <c r="X21" s="114"/>
+      <c r="Y21" s="114"/>
       <c r="Z21" s="18"/>
       <c r="AA21" s="19"/>
       <c r="AB21" s="13"/>
@@ -3531,7 +3540,7 @@
       <c r="BS21" s="6"/>
     </row>
     <row r="22" spans="2:71" x14ac:dyDescent="0.25">
-      <c r="B22" s="58"/>
+      <c r="B22" s="71"/>
       <c r="C22" s="13"/>
       <c r="D22" s="13"/>
       <c r="E22" s="13"/>
@@ -3556,33 +3565,33 @@
       <c r="X22" s="13"/>
       <c r="Y22" s="13"/>
       <c r="Z22" s="18"/>
-      <c r="AA22" s="70" t="s">
+      <c r="AA22" s="115" t="s">
         <v>94</v>
       </c>
-      <c r="AB22" s="69"/>
-      <c r="AC22" s="69"/>
-      <c r="AD22" s="69"/>
-      <c r="AE22" s="69"/>
-      <c r="AF22" s="69"/>
-      <c r="AG22" s="69"/>
-      <c r="AH22" s="69"/>
-      <c r="AI22" s="69"/>
-      <c r="AJ22" s="69"/>
-      <c r="AK22" s="69"/>
-      <c r="AL22" s="69"/>
-      <c r="AM22" s="69"/>
-      <c r="AN22" s="69"/>
-      <c r="AO22" s="69"/>
-      <c r="AP22" s="69"/>
-      <c r="AQ22" s="69"/>
-      <c r="AR22" s="69"/>
-      <c r="AS22" s="69"/>
-      <c r="AT22" s="69"/>
-      <c r="AU22" s="69"/>
-      <c r="AV22" s="69"/>
-      <c r="AW22" s="69"/>
-      <c r="AX22" s="69"/>
-      <c r="AY22" s="71"/>
+      <c r="AB22" s="114"/>
+      <c r="AC22" s="114"/>
+      <c r="AD22" s="114"/>
+      <c r="AE22" s="114"/>
+      <c r="AF22" s="114"/>
+      <c r="AG22" s="114"/>
+      <c r="AH22" s="114"/>
+      <c r="AI22" s="114"/>
+      <c r="AJ22" s="114"/>
+      <c r="AK22" s="114"/>
+      <c r="AL22" s="114"/>
+      <c r="AM22" s="114"/>
+      <c r="AN22" s="114"/>
+      <c r="AO22" s="114"/>
+      <c r="AP22" s="114"/>
+      <c r="AQ22" s="114"/>
+      <c r="AR22" s="114"/>
+      <c r="AS22" s="114"/>
+      <c r="AT22" s="114"/>
+      <c r="AU22" s="114"/>
+      <c r="AV22" s="114"/>
+      <c r="AW22" s="114"/>
+      <c r="AX22" s="114"/>
+      <c r="AY22" s="116"/>
       <c r="AZ22" s="12"/>
       <c r="BA22" s="12"/>
       <c r="BB22" s="12"/>
@@ -3605,7 +3614,7 @@
       <c r="BS22" s="6"/>
     </row>
     <row r="23" spans="2:71" x14ac:dyDescent="0.25">
-      <c r="B23" s="58"/>
+      <c r="B23" s="71"/>
       <c r="C23" s="13"/>
       <c r="D23" s="13"/>
       <c r="E23" s="13"/>
@@ -3658,7 +3667,7 @@
       <c r="BS23" s="6"/>
     </row>
     <row r="24" spans="2:71" x14ac:dyDescent="0.25">
-      <c r="B24" s="58"/>
+      <c r="B24" s="71"/>
       <c r="C24" s="13"/>
       <c r="D24" s="13"/>
       <c r="E24" s="13"/>
@@ -3685,27 +3694,27 @@
       <c r="Z24" s="18"/>
       <c r="AA24" s="19"/>
       <c r="AB24" s="13"/>
-      <c r="AC24" s="69" t="s">
+      <c r="AC24" s="114" t="s">
         <v>95</v>
       </c>
-      <c r="AD24" s="69"/>
-      <c r="AE24" s="69"/>
-      <c r="AF24" s="69"/>
-      <c r="AG24" s="69"/>
-      <c r="AH24" s="69"/>
-      <c r="AI24" s="69"/>
-      <c r="AJ24" s="69"/>
-      <c r="AK24" s="69"/>
-      <c r="AL24" s="69"/>
-      <c r="AM24" s="69"/>
-      <c r="AN24" s="69"/>
-      <c r="AO24" s="69"/>
-      <c r="AP24" s="69"/>
-      <c r="AQ24" s="69"/>
-      <c r="AR24" s="69"/>
-      <c r="AS24" s="69"/>
-      <c r="AT24" s="69"/>
-      <c r="AU24" s="69"/>
+      <c r="AD24" s="114"/>
+      <c r="AE24" s="114"/>
+      <c r="AF24" s="114"/>
+      <c r="AG24" s="114"/>
+      <c r="AH24" s="114"/>
+      <c r="AI24" s="114"/>
+      <c r="AJ24" s="114"/>
+      <c r="AK24" s="114"/>
+      <c r="AL24" s="114"/>
+      <c r="AM24" s="114"/>
+      <c r="AN24" s="114"/>
+      <c r="AO24" s="114"/>
+      <c r="AP24" s="114"/>
+      <c r="AQ24" s="114"/>
+      <c r="AR24" s="114"/>
+      <c r="AS24" s="114"/>
+      <c r="AT24" s="114"/>
+      <c r="AU24" s="114"/>
       <c r="AV24" s="12"/>
       <c r="AW24" s="12"/>
       <c r="AX24" s="12"/>
@@ -3732,7 +3741,7 @@
       <c r="BS24" s="6"/>
     </row>
     <row r="25" spans="2:71" x14ac:dyDescent="0.25">
-      <c r="B25" s="58"/>
+      <c r="B25" s="71"/>
       <c r="C25" s="13"/>
       <c r="D25" s="13"/>
       <c r="E25" s="13"/>
@@ -3782,31 +3791,31 @@
       <c r="AW25" s="12"/>
       <c r="AX25" s="12"/>
       <c r="AY25" s="25"/>
-      <c r="AZ25" s="70" t="s">
+      <c r="AZ25" s="115" t="s">
         <v>96</v>
       </c>
-      <c r="BA25" s="69"/>
-      <c r="BB25" s="69"/>
-      <c r="BC25" s="69"/>
-      <c r="BD25" s="69"/>
-      <c r="BE25" s="69"/>
-      <c r="BF25" s="69"/>
-      <c r="BG25" s="69"/>
-      <c r="BH25" s="69"/>
-      <c r="BI25" s="69"/>
-      <c r="BJ25" s="69"/>
-      <c r="BK25" s="69"/>
-      <c r="BL25" s="69"/>
-      <c r="BM25" s="69"/>
-      <c r="BN25" s="69"/>
-      <c r="BO25" s="69"/>
-      <c r="BP25" s="69"/>
+      <c r="BA25" s="114"/>
+      <c r="BB25" s="114"/>
+      <c r="BC25" s="114"/>
+      <c r="BD25" s="114"/>
+      <c r="BE25" s="114"/>
+      <c r="BF25" s="114"/>
+      <c r="BG25" s="114"/>
+      <c r="BH25" s="114"/>
+      <c r="BI25" s="114"/>
+      <c r="BJ25" s="114"/>
+      <c r="BK25" s="114"/>
+      <c r="BL25" s="114"/>
+      <c r="BM25" s="114"/>
+      <c r="BN25" s="114"/>
+      <c r="BO25" s="114"/>
+      <c r="BP25" s="114"/>
       <c r="BQ25" s="12"/>
       <c r="BR25" s="12"/>
       <c r="BS25" s="6"/>
     </row>
     <row r="26" spans="2:71" x14ac:dyDescent="0.25">
-      <c r="B26" s="58"/>
+      <c r="B26" s="71"/>
       <c r="C26" s="13"/>
       <c r="D26" s="13"/>
       <c r="E26" s="13"/>
@@ -3878,7 +3887,7 @@
       <c r="BS26" s="6"/>
     </row>
     <row r="27" spans="2:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="59"/>
+      <c r="B27" s="72"/>
       <c r="C27" s="14"/>
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
@@ -3950,18 +3959,10 @@
       <c r="BS27" s="7"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="CA18:CA23">
+    <sortCondition ref="CA18:CA23"/>
+  </sortState>
   <mergeCells count="27">
-    <mergeCell ref="AZ25:BP25"/>
-    <mergeCell ref="F11:S11"/>
-    <mergeCell ref="I13:W13"/>
-    <mergeCell ref="J15:U15"/>
-    <mergeCell ref="K17:W17"/>
-    <mergeCell ref="K19:X19"/>
-    <mergeCell ref="AU4:AY4"/>
-    <mergeCell ref="AA6:AY6"/>
-    <mergeCell ref="K21:Y21"/>
-    <mergeCell ref="AA22:AY22"/>
-    <mergeCell ref="AC24:AU24"/>
     <mergeCell ref="B7:B27"/>
     <mergeCell ref="C7:N7"/>
     <mergeCell ref="F9:O9"/>
@@ -3978,6 +3979,17 @@
     <mergeCell ref="AF4:AJ4"/>
     <mergeCell ref="AK4:AO4"/>
     <mergeCell ref="AP4:AT4"/>
+    <mergeCell ref="AU4:AY4"/>
+    <mergeCell ref="AA6:AY6"/>
+    <mergeCell ref="K21:Y21"/>
+    <mergeCell ref="AA22:AY22"/>
+    <mergeCell ref="AC24:AU24"/>
+    <mergeCell ref="AZ25:BP25"/>
+    <mergeCell ref="F11:S11"/>
+    <mergeCell ref="I13:W13"/>
+    <mergeCell ref="J15:U15"/>
+    <mergeCell ref="K17:W17"/>
+    <mergeCell ref="K19:X19"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -4000,81 +4012,81 @@
   </cols>
   <sheetData>
     <row r="6" spans="3:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="C6" s="73" t="s">
+      <c r="C6" s="79" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" s="79"/>
+      <c r="E6" s="79"/>
+      <c r="F6" s="79"/>
+      <c r="G6" s="79"/>
+      <c r="H6" s="79"/>
+      <c r="I6" s="79"/>
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C7" s="80" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" s="80"/>
+      <c r="E7" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="F7" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="D6" s="73"/>
-      <c r="E6" s="73"/>
-      <c r="F6" s="73"/>
-      <c r="G6" s="73"/>
-      <c r="H6" s="73"/>
-      <c r="I6" s="73"/>
-    </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C7" s="74" t="s">
-        <v>100</v>
-      </c>
-      <c r="D7" s="74"/>
-      <c r="E7" s="28" t="s">
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C8" s="78" t="s">
         <v>102</v>
       </c>
-      <c r="F7" s="28" t="s">
+      <c r="D8" s="78"/>
+      <c r="E8" s="31" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C8" s="72" t="s">
+      <c r="F8" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="72"/>
-      <c r="E8" s="31" t="s">
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C9" s="78" t="s">
         <v>105</v>
       </c>
-      <c r="F8" s="31" t="s">
+      <c r="D9" s="78"/>
+      <c r="E9" s="31" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C9" s="72" t="s">
+      <c r="F9" s="31" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C10" s="78" t="s">
         <v>107</v>
       </c>
-      <c r="D9" s="72"/>
-      <c r="E9" s="31" t="s">
+      <c r="D10" s="78"/>
+      <c r="E10" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="F9" s="31" t="s">
+      <c r="F10" s="31" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C10" s="72" t="s">
+    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C11" s="78" t="s">
         <v>109</v>
       </c>
-      <c r="D10" s="72"/>
-      <c r="E10" s="31" t="s">
+      <c r="D11" s="78"/>
+      <c r="E11" s="31" t="s">
         <v>110</v>
-      </c>
-      <c r="F10" s="31" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C11" s="72" t="s">
-        <v>111</v>
-      </c>
-      <c r="D11" s="72"/>
-      <c r="E11" s="31" t="s">
-        <v>112</v>
       </c>
       <c r="F11" s="31" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="12" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C12" s="72" t="s">
-        <v>113</v>
-      </c>
-      <c r="D12" s="72"/>
+      <c r="C12" s="78" t="s">
+        <v>111</v>
+      </c>
+      <c r="D12" s="78"/>
       <c r="E12" s="31" t="s">
         <v>56</v>
       </c>
@@ -4083,103 +4095,122 @@
       </c>
     </row>
     <row r="13" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C13" s="72"/>
-      <c r="D13" s="72"/>
+      <c r="C13" s="78"/>
+      <c r="D13" s="78"/>
     </row>
     <row r="14" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C14" s="72"/>
-      <c r="D14" s="72"/>
+      <c r="C14" s="78"/>
+      <c r="D14" s="78"/>
     </row>
     <row r="15" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C15" s="72"/>
-      <c r="D15" s="72"/>
+      <c r="C15" s="78"/>
+      <c r="D15" s="78"/>
     </row>
     <row r="16" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C16" s="72"/>
-      <c r="D16" s="72"/>
+      <c r="C16" s="78"/>
+      <c r="D16" s="78"/>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C17" s="72"/>
-      <c r="D17" s="72"/>
+      <c r="C17" s="78"/>
+      <c r="D17" s="78"/>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C18" s="72"/>
-      <c r="D18" s="72"/>
+      <c r="C18" s="78"/>
+      <c r="D18" s="78"/>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C19" s="72"/>
-      <c r="D19" s="72"/>
+      <c r="C19" s="78"/>
+      <c r="D19" s="78"/>
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C20" s="72"/>
-      <c r="D20" s="72"/>
+      <c r="C20" s="78"/>
+      <c r="D20" s="78"/>
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C21" s="72"/>
-      <c r="D21" s="72"/>
+      <c r="C21" s="78"/>
+      <c r="D21" s="78"/>
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C22" s="72"/>
-      <c r="D22" s="72"/>
+      <c r="C22" s="78"/>
+      <c r="D22" s="78"/>
     </row>
     <row r="23" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C23" s="72"/>
-      <c r="D23" s="72"/>
+      <c r="C23" s="78"/>
+      <c r="D23" s="78"/>
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C24" s="72"/>
-      <c r="D24" s="72"/>
+      <c r="C24" s="78"/>
+      <c r="D24" s="78"/>
     </row>
     <row r="25" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C25" s="72"/>
-      <c r="D25" s="72"/>
+      <c r="C25" s="78"/>
+      <c r="D25" s="78"/>
     </row>
     <row r="26" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C26" s="72"/>
-      <c r="D26" s="72"/>
+      <c r="C26" s="78"/>
+      <c r="D26" s="78"/>
     </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C27" s="72"/>
-      <c r="D27" s="72"/>
+      <c r="C27" s="78"/>
+      <c r="D27" s="78"/>
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C28" s="72"/>
-      <c r="D28" s="72"/>
+      <c r="C28" s="78"/>
+      <c r="D28" s="78"/>
     </row>
     <row r="29" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C29" s="72"/>
-      <c r="D29" s="72"/>
+      <c r="C29" s="78"/>
+      <c r="D29" s="78"/>
     </row>
     <row r="30" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C30" s="72"/>
-      <c r="D30" s="72"/>
+      <c r="C30" s="78"/>
+      <c r="D30" s="78"/>
     </row>
     <row r="31" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C31" s="72"/>
-      <c r="D31" s="72"/>
+      <c r="C31" s="78"/>
+      <c r="D31" s="78"/>
     </row>
     <row r="32" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C32" s="72"/>
-      <c r="D32" s="72"/>
+      <c r="C32" s="78"/>
+      <c r="D32" s="78"/>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C33" s="72"/>
-      <c r="D33" s="72"/>
+      <c r="C33" s="78"/>
+      <c r="D33" s="78"/>
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C34" s="72"/>
-      <c r="D34" s="72"/>
+      <c r="C34" s="78"/>
+      <c r="D34" s="78"/>
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C35" s="72"/>
-      <c r="D35" s="72"/>
+      <c r="C35" s="78"/>
+      <c r="D35" s="78"/>
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C36" s="72"/>
-      <c r="D36" s="72"/>
+      <c r="C36" s="78"/>
+      <c r="D36" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C6:I6"/>
     <mergeCell ref="C7:D7"/>
@@ -4192,25 +4223,6 @@
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -4221,7 +4233,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3966DD9C-32B9-42AC-8D7D-E5F84A7C120D}">
   <dimension ref="C1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
@@ -4256,12 +4268,12 @@
     </row>
     <row r="4" spans="3:9" ht="21" x14ac:dyDescent="0.25">
       <c r="C4" s="49"/>
-      <c r="D4" s="108"/>
+      <c r="D4" s="57"/>
       <c r="E4" s="49"/>
-      <c r="F4" s="107"/>
-      <c r="G4" s="107"/>
-      <c r="H4" s="107"/>
-      <c r="I4" s="107"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C5" s="51"/>
@@ -4275,420 +4287,420 @@
     <row r="7" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="52" t="s">
-        <v>156</v>
-      </c>
-      <c r="D8" s="109" t="s">
-        <v>121</v>
+        <v>154</v>
+      </c>
+      <c r="D8" s="58" t="s">
+        <v>119</v>
       </c>
       <c r="E8" s="53" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="113" t="s">
+      <c r="C9" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="114"/>
-      <c r="E9" s="115"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="64"/>
     </row>
     <row r="10" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C10" s="111">
+      <c r="C10" s="60">
         <v>1</v>
       </c>
-      <c r="D10" s="112" t="s">
+      <c r="D10" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="111" t="s">
+      <c r="E10" s="60" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="11" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C11" s="110">
+      <c r="C11" s="59">
         <v>2</v>
       </c>
       <c r="D11" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="110" t="s">
-        <v>193</v>
+      <c r="E11" s="59" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="12" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C12" s="110">
+      <c r="C12" s="59">
         <v>3</v>
       </c>
       <c r="D12" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="110" t="s">
-        <v>192</v>
+      <c r="E12" s="59" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="13" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C13" s="110">
+      <c r="C13" s="59">
         <v>4</v>
       </c>
       <c r="D13" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="110" t="s">
-        <v>192</v>
+      <c r="E13" s="59" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="14" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C14" s="110">
+      <c r="C14" s="59">
         <v>5</v>
       </c>
       <c r="D14" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="110" t="s">
+      <c r="E14" s="59" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="15" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C15" s="110">
+      <c r="C15" s="59">
         <v>6</v>
       </c>
       <c r="D15" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="110" t="s">
-        <v>191</v>
+      <c r="E15" s="59" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="16" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C16" s="110">
+      <c r="C16" s="59">
         <v>7</v>
       </c>
       <c r="D16" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="110" t="s">
-        <v>190</v>
+      <c r="E16" s="59" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C17" s="110">
+      <c r="C17" s="59">
         <v>8</v>
       </c>
       <c r="D17" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="110" t="s">
+      <c r="E17" s="59" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C18" s="110">
+      <c r="C18" s="59">
         <v>9</v>
       </c>
       <c r="D18" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="110" t="s">
-        <v>184</v>
+      <c r="E18" s="59" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="19" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="116" t="s">
+      <c r="C19" s="65" t="s">
         <v>4</v>
       </c>
       <c r="D19" s="55"/>
-      <c r="E19" s="117"/>
+      <c r="E19" s="66"/>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C20" s="111">
+      <c r="C20" s="60">
         <v>1</v>
       </c>
-      <c r="D20" s="112" t="s">
+      <c r="D20" s="61" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="111" t="s">
-        <v>189</v>
+      <c r="E20" s="60" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C21" s="110">
+      <c r="C21" s="59">
         <v>2</v>
       </c>
       <c r="D21" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="E21" s="110" t="s">
-        <v>188</v>
+      <c r="E21" s="59" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C22" s="110">
+      <c r="C22" s="59">
         <v>3</v>
       </c>
       <c r="D22" s="54" t="s">
         <v>57</v>
       </c>
-      <c r="E22" s="110" t="s">
-        <v>182</v>
+      <c r="E22" s="59" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C23" s="110">
+      <c r="C23" s="59">
         <v>4</v>
       </c>
       <c r="D23" s="54" t="s">
-        <v>167</v>
-      </c>
-      <c r="E23" s="110" t="s">
-        <v>187</v>
+        <v>165</v>
+      </c>
+      <c r="E23" s="59" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C24" s="110">
+      <c r="C24" s="59">
         <v>5</v>
       </c>
       <c r="D24" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="E24" s="110"/>
+      <c r="E24" s="59"/>
     </row>
     <row r="25" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="116" t="s">
+      <c r="C25" s="65" t="s">
+        <v>166</v>
+      </c>
+      <c r="D25" s="55"/>
+      <c r="E25" s="66"/>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C26" s="60">
+        <v>1</v>
+      </c>
+      <c r="D26" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="E26" s="60" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C27" s="59">
+        <v>2</v>
+      </c>
+      <c r="D27" s="54" t="s">
+        <v>167</v>
+      </c>
+      <c r="E27" s="59" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C28" s="59">
+        <v>3</v>
+      </c>
+      <c r="D28" s="54" t="s">
         <v>168</v>
       </c>
-      <c r="D25" s="55"/>
-      <c r="E25" s="117"/>
-    </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C26" s="111">
-        <v>1</v>
-      </c>
-      <c r="D26" s="112" t="s">
-        <v>54</v>
-      </c>
-      <c r="E26" s="111" t="s">
+      <c r="E28" s="59" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C27" s="110">
-        <v>2</v>
-      </c>
-      <c r="D27" s="54" t="s">
+    <row r="29" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C29" s="59">
+        <v>4</v>
+      </c>
+      <c r="D29" s="54" t="s">
         <v>169</v>
       </c>
-      <c r="E27" s="110" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C28" s="110">
-        <v>3</v>
-      </c>
-      <c r="D28" s="54" t="s">
-        <v>170</v>
-      </c>
-      <c r="E28" s="110" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="29" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C29" s="110">
-        <v>4</v>
-      </c>
-      <c r="D29" s="54" t="s">
+      <c r="E29" s="59" t="s">
         <v>171</v>
       </c>
-      <c r="E29" s="110" t="s">
-        <v>173</v>
-      </c>
     </row>
     <row r="30" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C30" s="110">
+      <c r="C30" s="59">
         <v>5</v>
       </c>
       <c r="D30" s="54" t="s">
-        <v>109</v>
-      </c>
-      <c r="E30" s="110" t="s">
-        <v>185</v>
+        <v>107</v>
+      </c>
+      <c r="E30" s="59" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="31" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C31" s="110">
+      <c r="C31" s="59">
         <v>6</v>
       </c>
       <c r="D31" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="E31" s="110" t="s">
+      <c r="E31" s="59" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="32" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C32" s="59">
+        <v>7</v>
+      </c>
+      <c r="D32" s="54" t="s">
+        <v>170</v>
+      </c>
+      <c r="E32" s="59" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C33" s="65" t="s">
+        <v>3</v>
+      </c>
+      <c r="D33" s="55"/>
+      <c r="E33" s="66"/>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C34" s="60">
+        <v>1</v>
+      </c>
+      <c r="D34" s="61" t="s">
+        <v>156</v>
+      </c>
+      <c r="E34" s="60" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="32" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C32" s="110">
-        <v>7</v>
-      </c>
-      <c r="D32" s="54" t="s">
-        <v>172</v>
-      </c>
-      <c r="E32" s="110" t="s">
+    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C35" s="59">
+        <v>2</v>
+      </c>
+      <c r="D35" s="54" t="s">
+        <v>157</v>
+      </c>
+      <c r="E35" s="59" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="33" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C33" s="116" t="s">
+    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C36" s="59">
         <v>3</v>
       </c>
-      <c r="D33" s="55"/>
-      <c r="E33" s="117"/>
-    </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C34" s="111">
-        <v>1</v>
-      </c>
-      <c r="D34" s="112" t="s">
+      <c r="D36" s="54" t="s">
         <v>158</v>
       </c>
-      <c r="E34" s="111" t="s">
+      <c r="E36" s="59" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C35" s="110">
-        <v>2</v>
-      </c>
-      <c r="D35" s="54" t="s">
+    <row r="37" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C37" s="59">
+        <v>4</v>
+      </c>
+      <c r="D37" s="54" t="s">
         <v>159</v>
       </c>
-      <c r="E35" s="110" t="s">
+      <c r="E37" s="59" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C38" s="59">
+        <v>5</v>
+      </c>
+      <c r="D38" s="54" t="s">
+        <v>170</v>
+      </c>
+      <c r="E38" s="59" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C36" s="110">
-        <v>3</v>
-      </c>
-      <c r="D36" s="54" t="s">
-        <v>160</v>
-      </c>
-      <c r="E36" s="110" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="37" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C37" s="110">
-        <v>4</v>
-      </c>
-      <c r="D37" s="54" t="s">
-        <v>161</v>
-      </c>
-      <c r="E37" s="110" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C38" s="110">
-        <v>5</v>
-      </c>
-      <c r="D38" s="54" t="s">
-        <v>172</v>
-      </c>
-      <c r="E38" s="110" t="s">
-        <v>179</v>
-      </c>
-    </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C39" s="110">
+      <c r="C39" s="59">
         <v>6</v>
       </c>
       <c r="D39" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="E39" s="110" t="s">
-        <v>184</v>
+      <c r="E39" s="59" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="40" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C40" s="110">
+      <c r="C40" s="59">
         <v>7</v>
       </c>
       <c r="D40" s="54" t="s">
-        <v>107</v>
-      </c>
-      <c r="E40" s="110" t="s">
-        <v>180</v>
+        <v>105</v>
+      </c>
+      <c r="E40" s="59" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="41" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C41" s="116" t="s">
-        <v>129</v>
+      <c r="C41" s="65" t="s">
+        <v>127</v>
       </c>
       <c r="D41" s="55"/>
-      <c r="E41" s="117"/>
+      <c r="E41" s="66"/>
     </row>
     <row r="42" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C42" s="111">
+      <c r="C42" s="60">
         <v>1</v>
       </c>
-      <c r="D42" s="112" t="s">
+      <c r="D42" s="61" t="s">
+        <v>160</v>
+      </c>
+      <c r="E42" s="60" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C43" s="59">
+        <v>2</v>
+      </c>
+      <c r="D43" s="54" t="s">
+        <v>161</v>
+      </c>
+      <c r="E43" s="59" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="44" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C44" s="59">
+        <v>3</v>
+      </c>
+      <c r="D44" s="54" t="s">
         <v>162</v>
       </c>
-      <c r="E42" s="111" t="s">
+      <c r="E44" s="59" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C43" s="110">
-        <v>2</v>
-      </c>
-      <c r="D43" s="54" t="s">
+    <row r="45" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C45" s="59">
+        <v>4</v>
+      </c>
+      <c r="D45" s="54" t="s">
         <v>163</v>
       </c>
-      <c r="E43" s="110" t="s">
+      <c r="E45" s="59" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="46" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C46" s="59">
+        <v>5</v>
+      </c>
+      <c r="D46" s="54" t="s">
+        <v>164</v>
+      </c>
+      <c r="E46" s="59" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="44" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C44" s="110">
-        <v>3</v>
-      </c>
-      <c r="D44" s="54" t="s">
-        <v>164</v>
-      </c>
-      <c r="E44" s="110" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="45" spans="3:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="C45" s="110">
-        <v>4</v>
-      </c>
-      <c r="D45" s="54" t="s">
-        <v>165</v>
-      </c>
-      <c r="E45" s="110" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="46" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C46" s="110">
-        <v>5</v>
-      </c>
-      <c r="D46" s="54" t="s">
-        <v>166</v>
-      </c>
-      <c r="E46" s="110" t="s">
-        <v>183</v>
-      </c>
-    </row>
     <row r="47" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C47" s="110">
+      <c r="C47" s="59">
         <v>6</v>
       </c>
       <c r="D47" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="E47" s="110" t="s">
-        <v>182</v>
+      <c r="E47" s="59" t="s">
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -4804,78 +4816,78 @@
       </c>
     </row>
     <row r="12" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D12" s="75" t="s">
+      <c r="D12" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="75"/>
-      <c r="F12" s="75"/>
-      <c r="G12" s="75"/>
-      <c r="H12" s="75"/>
-      <c r="I12" s="75"/>
+      <c r="E12" s="81"/>
+      <c r="F12" s="81"/>
+      <c r="G12" s="81"/>
+      <c r="H12" s="81"/>
+      <c r="I12" s="81"/>
     </row>
     <row r="13" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D13" s="75"/>
-      <c r="E13" s="75"/>
-      <c r="F13" s="75"/>
-      <c r="G13" s="75"/>
-      <c r="H13" s="75"/>
-      <c r="I13" s="75"/>
+      <c r="D13" s="81"/>
+      <c r="E13" s="81"/>
+      <c r="F13" s="81"/>
+      <c r="G13" s="81"/>
+      <c r="H13" s="81"/>
+      <c r="I13" s="81"/>
     </row>
     <row r="14" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D14" s="75"/>
-      <c r="E14" s="75"/>
-      <c r="F14" s="75"/>
-      <c r="G14" s="75"/>
-      <c r="H14" s="75"/>
-      <c r="I14" s="75"/>
+      <c r="D14" s="81"/>
+      <c r="E14" s="81"/>
+      <c r="F14" s="81"/>
+      <c r="G14" s="81"/>
+      <c r="H14" s="81"/>
+      <c r="I14" s="81"/>
     </row>
     <row r="15" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D15" s="75"/>
-      <c r="E15" s="75"/>
-      <c r="F15" s="75"/>
-      <c r="G15" s="75"/>
-      <c r="H15" s="75"/>
-      <c r="I15" s="75"/>
+      <c r="D15" s="81"/>
+      <c r="E15" s="81"/>
+      <c r="F15" s="81"/>
+      <c r="G15" s="81"/>
+      <c r="H15" s="81"/>
+      <c r="I15" s="81"/>
     </row>
     <row r="16" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D16" s="75"/>
-      <c r="E16" s="75"/>
-      <c r="F16" s="75"/>
-      <c r="G16" s="75"/>
-      <c r="H16" s="75"/>
-      <c r="I16" s="75"/>
+      <c r="D16" s="81"/>
+      <c r="E16" s="81"/>
+      <c r="F16" s="81"/>
+      <c r="G16" s="81"/>
+      <c r="H16" s="81"/>
+      <c r="I16" s="81"/>
     </row>
     <row r="17" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D17" s="75"/>
-      <c r="E17" s="75"/>
-      <c r="F17" s="75"/>
-      <c r="G17" s="75"/>
-      <c r="H17" s="75"/>
-      <c r="I17" s="75"/>
+      <c r="D17" s="81"/>
+      <c r="E17" s="81"/>
+      <c r="F17" s="81"/>
+      <c r="G17" s="81"/>
+      <c r="H17" s="81"/>
+      <c r="I17" s="81"/>
     </row>
     <row r="18" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D18" s="75"/>
-      <c r="E18" s="75"/>
-      <c r="F18" s="75"/>
-      <c r="G18" s="75"/>
-      <c r="H18" s="75"/>
-      <c r="I18" s="75"/>
+      <c r="D18" s="81"/>
+      <c r="E18" s="81"/>
+      <c r="F18" s="81"/>
+      <c r="G18" s="81"/>
+      <c r="H18" s="81"/>
+      <c r="I18" s="81"/>
     </row>
     <row r="19" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D19" s="75"/>
-      <c r="E19" s="75"/>
-      <c r="F19" s="75"/>
-      <c r="G19" s="75"/>
-      <c r="H19" s="75"/>
-      <c r="I19" s="75"/>
+      <c r="D19" s="81"/>
+      <c r="E19" s="81"/>
+      <c r="F19" s="81"/>
+      <c r="G19" s="81"/>
+      <c r="H19" s="81"/>
+      <c r="I19" s="81"/>
     </row>
     <row r="20" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D20" s="75"/>
-      <c r="E20" s="75"/>
-      <c r="F20" s="75"/>
-      <c r="G20" s="75"/>
-      <c r="H20" s="75"/>
-      <c r="I20" s="75"/>
+      <c r="D20" s="81"/>
+      <c r="E20" s="81"/>
+      <c r="F20" s="81"/>
+      <c r="G20" s="81"/>
+      <c r="H20" s="81"/>
+      <c r="I20" s="81"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4947,7 +4959,7 @@
         <v>61</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>0</v>
@@ -4956,7 +4968,7 @@
         <v>41</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
@@ -5100,13 +5112,13 @@
         <v>64</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>0</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
@@ -5251,37 +5263,37 @@
   <sheetData>
     <row r="3" spans="4:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="4:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D4" s="95" t="s">
-        <v>132</v>
-      </c>
-      <c r="E4" s="96"/>
-      <c r="F4" s="96"/>
-      <c r="G4" s="96"/>
-      <c r="H4" s="96"/>
-      <c r="I4" s="96"/>
-      <c r="J4" s="96"/>
-      <c r="K4" s="97"/>
-      <c r="M4" s="92" t="s">
-        <v>138</v>
-      </c>
-      <c r="N4" s="93"/>
-      <c r="O4" s="93"/>
-      <c r="P4" s="93"/>
-      <c r="Q4" s="93"/>
-      <c r="R4" s="93"/>
-      <c r="S4" s="93"/>
-      <c r="T4" s="93"/>
-      <c r="U4" s="94"/>
+      <c r="D4" s="85" t="s">
+        <v>130</v>
+      </c>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="86"/>
+      <c r="I4" s="86"/>
+      <c r="J4" s="86"/>
+      <c r="K4" s="87"/>
+      <c r="M4" s="82" t="s">
+        <v>136</v>
+      </c>
+      <c r="N4" s="83"/>
+      <c r="O4" s="83"/>
+      <c r="P4" s="83"/>
+      <c r="Q4" s="83"/>
+      <c r="R4" s="83"/>
+      <c r="S4" s="83"/>
+      <c r="T4" s="83"/>
+      <c r="U4" s="84"/>
     </row>
     <row r="5" spans="4:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D5" s="45" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E5" s="45" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F5" s="46" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G5" s="47">
         <v>100</v>
@@ -5299,31 +5311,31 @@
         <v>1700</v>
       </c>
       <c r="M5" s="40" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="N5" s="40" t="s">
+        <v>131</v>
+      </c>
+      <c r="O5" s="40" t="s">
+        <v>132</v>
+      </c>
+      <c r="P5" s="40" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q5" s="40" t="s">
         <v>133</v>
       </c>
-      <c r="O5" s="40" t="s">
+      <c r="R5" s="40" t="s">
         <v>134</v>
       </c>
-      <c r="P5" s="40" t="s">
+      <c r="S5" s="40" t="s">
+        <v>135</v>
+      </c>
+      <c r="T5" s="40" t="s">
         <v>140</v>
       </c>
-      <c r="Q5" s="40" t="s">
-        <v>135</v>
-      </c>
-      <c r="R5" s="40" t="s">
-        <v>136</v>
-      </c>
-      <c r="S5" s="40" t="s">
-        <v>137</v>
-      </c>
-      <c r="T5" s="40" t="s">
-        <v>142</v>
-      </c>
       <c r="U5" s="40" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="4:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -5331,7 +5343,7 @@
         <v>0.4</v>
       </c>
       <c r="E6" s="38" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F6" s="43">
         <f>U6</f>
@@ -5364,7 +5376,7 @@
         <v>40</v>
       </c>
       <c r="O6" s="38" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="P6" s="38">
         <v>80</v>
@@ -5379,7 +5391,7 @@
         <v>75</v>
       </c>
       <c r="T6" s="38" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="U6" s="38">
         <f>(N6/P6)*(P6/Q6)*(R6/S6)</f>
@@ -5391,7 +5403,7 @@
         <v>0.5</v>
       </c>
       <c r="E7" s="38" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F7" s="43">
         <f>U7</f>
@@ -5424,7 +5436,7 @@
         <v>40</v>
       </c>
       <c r="O7" s="38" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="P7" s="38">
         <v>80</v>
@@ -5439,7 +5451,7 @@
         <v>80</v>
       </c>
       <c r="T7" s="38" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="U7" s="38">
         <f t="shared" ref="U7:U24" si="5">(N7/P7)*(P7/Q7)*(R7/S7)</f>
@@ -5451,7 +5463,7 @@
         <v>0.7</v>
       </c>
       <c r="E8" s="38" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F8" s="43">
         <f t="shared" ref="F8:F26" si="6">U8</f>
@@ -5484,7 +5496,7 @@
         <v>40</v>
       </c>
       <c r="O8" s="38" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="P8" s="38">
         <v>80</v>
@@ -5499,7 +5511,7 @@
         <v>50</v>
       </c>
       <c r="T8" s="38" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="U8" s="38">
         <f t="shared" si="5"/>
@@ -5511,7 +5523,7 @@
         <v>0.8</v>
       </c>
       <c r="E9" s="38" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F9" s="43">
         <f t="shared" si="6"/>
@@ -5544,7 +5556,7 @@
         <v>40</v>
       </c>
       <c r="O9" s="38" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="P9" s="38">
         <v>80</v>
@@ -5559,7 +5571,7 @@
         <v>50</v>
       </c>
       <c r="T9" s="38" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="U9" s="38">
         <f t="shared" si="5"/>
@@ -5571,7 +5583,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="38" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F10" s="43">
         <f t="shared" si="6"/>
@@ -5604,7 +5616,7 @@
         <v>40</v>
       </c>
       <c r="O10" s="38" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="P10" s="38">
         <v>80</v>
@@ -5619,7 +5631,7 @@
         <v>75</v>
       </c>
       <c r="T10" s="38" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="U10" s="38">
         <f t="shared" si="5"/>
@@ -5631,7 +5643,7 @@
         <v>1.25</v>
       </c>
       <c r="E11" s="38" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F11" s="43">
         <f t="shared" si="6"/>
@@ -5664,7 +5676,7 @@
         <v>40</v>
       </c>
       <c r="O11" s="38" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="P11" s="38">
         <v>80</v>
@@ -5679,7 +5691,7 @@
         <v>60</v>
       </c>
       <c r="T11" s="38" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="U11" s="38">
         <f t="shared" si="5"/>
@@ -5691,7 +5703,7 @@
         <v>1.5</v>
       </c>
       <c r="E12" s="38" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F12" s="43">
         <f t="shared" si="6"/>
@@ -5724,7 +5736,7 @@
         <v>40</v>
       </c>
       <c r="O12" s="38" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="P12" s="38">
         <v>80</v>
@@ -5739,7 +5751,7 @@
         <v>50</v>
       </c>
       <c r="T12" s="38" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="U12" s="38">
         <f t="shared" si="5"/>
@@ -5751,7 +5763,7 @@
         <v>1.75</v>
       </c>
       <c r="E13" s="38" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F13" s="43">
         <f t="shared" si="6"/>
@@ -5784,7 +5796,7 @@
         <v>40</v>
       </c>
       <c r="O13" s="38" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="P13" s="38">
         <v>80</v>
@@ -5799,7 +5811,7 @@
         <v>40</v>
       </c>
       <c r="T13" s="38" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="U13" s="38">
         <f t="shared" si="5"/>
@@ -5811,7 +5823,7 @@
         <v>2</v>
       </c>
       <c r="E14" s="38" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F14" s="43">
         <f t="shared" si="6"/>
@@ -5844,7 +5856,7 @@
         <v>40</v>
       </c>
       <c r="O14" s="38" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="P14" s="38">
         <v>80</v>
@@ -5859,7 +5871,7 @@
         <v>40</v>
       </c>
       <c r="T14" s="38" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="U14" s="38">
         <f t="shared" si="5"/>
@@ -5871,7 +5883,7 @@
         <v>2.5</v>
       </c>
       <c r="E15" s="38" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F15" s="43">
         <f t="shared" si="6"/>
@@ -5904,7 +5916,7 @@
         <v>40</v>
       </c>
       <c r="O15" s="38" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="P15" s="38">
         <v>80</v>
@@ -5919,7 +5931,7 @@
         <v>30</v>
       </c>
       <c r="T15" s="38" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="U15" s="38">
         <f t="shared" si="5"/>
@@ -5931,7 +5943,7 @@
         <v>3</v>
       </c>
       <c r="E16" s="38" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F16" s="43">
         <f t="shared" si="6"/>
@@ -5964,7 +5976,7 @@
         <v>40</v>
       </c>
       <c r="O16" s="38" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="P16" s="38">
         <v>80</v>
@@ -5979,7 +5991,7 @@
         <v>25</v>
       </c>
       <c r="T16" s="38" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="U16" s="38">
         <f t="shared" si="5"/>
@@ -5991,7 +6003,7 @@
         <v>10</v>
       </c>
       <c r="E17" s="38" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F17" s="43">
         <f t="shared" si="6"/>
@@ -6024,7 +6036,7 @@
         <v>40</v>
       </c>
       <c r="O17" s="38" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="P17" s="38">
         <v>80</v>
@@ -6039,7 +6051,7 @@
         <v>65</v>
       </c>
       <c r="T17" s="38" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="U17" s="38">
         <f t="shared" si="5"/>
@@ -6051,7 +6063,7 @@
         <v>11</v>
       </c>
       <c r="E18" s="38" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F18" s="43">
         <f t="shared" si="6"/>
@@ -6084,7 +6096,7 @@
         <v>40</v>
       </c>
       <c r="O18" s="38" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="P18" s="38">
         <v>80</v>
@@ -6099,7 +6111,7 @@
         <v>65</v>
       </c>
       <c r="T18" s="38" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="U18" s="38">
         <f t="shared" si="5"/>
@@ -6111,7 +6123,7 @@
         <v>13</v>
       </c>
       <c r="E19" s="38" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F19" s="43">
         <f t="shared" si="6"/>
@@ -6144,7 +6156,7 @@
         <v>40</v>
       </c>
       <c r="O19" s="38" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="P19" s="38">
         <v>80</v>
@@ -6159,7 +6171,7 @@
         <v>50</v>
       </c>
       <c r="T19" s="38" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="U19" s="38">
         <f t="shared" si="5"/>
@@ -6171,7 +6183,7 @@
         <v>19</v>
       </c>
       <c r="E20" s="38" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F20" s="43">
         <f t="shared" si="6"/>
@@ -6204,7 +6216,7 @@
         <v>40</v>
       </c>
       <c r="O20" s="38" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="P20" s="38">
         <v>80</v>
@@ -6219,7 +6231,7 @@
         <v>75</v>
       </c>
       <c r="T20" s="38" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="U20" s="38">
         <f t="shared" si="5"/>
@@ -6231,7 +6243,7 @@
         <v>20</v>
       </c>
       <c r="E21" s="38" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F21" s="43">
         <f t="shared" si="6"/>
@@ -6264,7 +6276,7 @@
         <v>40</v>
       </c>
       <c r="O21" s="38" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="P21" s="38">
         <v>80</v>
@@ -6279,7 +6291,7 @@
         <v>65</v>
       </c>
       <c r="T21" s="38" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="U21" s="38">
         <f t="shared" si="5"/>
@@ -6291,7 +6303,7 @@
         <v>22</v>
       </c>
       <c r="E22" s="38" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F22" s="43">
         <f t="shared" si="6"/>
@@ -6324,7 +6336,7 @@
         <v>40</v>
       </c>
       <c r="O22" s="38" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="P22" s="38">
         <v>80</v>
@@ -6339,7 +6351,7 @@
         <v>65</v>
       </c>
       <c r="T22" s="38" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="U22" s="38">
         <f t="shared" si="5"/>
@@ -6351,7 +6363,7 @@
         <v>40</v>
       </c>
       <c r="E23" s="38" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F23" s="43">
         <f t="shared" si="6"/>
@@ -6384,7 +6396,7 @@
         <v>40</v>
       </c>
       <c r="O23" s="38" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="P23" s="38">
         <v>50</v>
@@ -6399,7 +6411,7 @@
         <v>65</v>
       </c>
       <c r="T23" s="38" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="U23" s="38">
         <f t="shared" si="5"/>
@@ -6411,7 +6423,7 @@
         <v>44</v>
       </c>
       <c r="E24" s="38" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F24" s="43">
         <f t="shared" si="6"/>
@@ -6444,7 +6456,7 @@
         <v>40</v>
       </c>
       <c r="O24" s="38" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="P24" s="38">
         <v>60</v>
@@ -6459,7 +6471,7 @@
         <v>65</v>
       </c>
       <c r="T24" s="38" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="U24" s="38">
         <f t="shared" si="5"/>
@@ -6471,7 +6483,7 @@
         <v>0.09</v>
       </c>
       <c r="E25" s="38" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F25" s="43">
         <f t="shared" si="6"/>
@@ -6519,7 +6531,7 @@
         <v>80</v>
       </c>
       <c r="T25" s="38" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="U25" s="38">
         <f>(N25/O25)*(P25/Q25)*(R25/S25)</f>
@@ -6531,7 +6543,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="E26" s="39" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F26" s="44">
         <f t="shared" si="6"/>
@@ -6579,7 +6591,7 @@
         <v>80</v>
       </c>
       <c r="T26" s="39" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="U26" s="39">
         <f>(N26/O26)*(P26/Q26)*(R26/S26)</f>
@@ -6588,237 +6600,242 @@
     </row>
     <row r="27" spans="4:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="4:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D28" s="95" t="s">
-        <v>155</v>
-      </c>
-      <c r="E28" s="96"/>
-      <c r="F28" s="96"/>
-      <c r="G28" s="96"/>
-      <c r="H28" s="96"/>
-      <c r="I28" s="96"/>
-      <c r="J28" s="96"/>
-      <c r="K28" s="96"/>
-      <c r="L28" s="97"/>
+      <c r="D28" s="85" t="s">
+        <v>153</v>
+      </c>
+      <c r="E28" s="86"/>
+      <c r="F28" s="86"/>
+      <c r="G28" s="86"/>
+      <c r="H28" s="86"/>
+      <c r="I28" s="86"/>
+      <c r="J28" s="86"/>
+      <c r="K28" s="86"/>
+      <c r="L28" s="87"/>
     </row>
     <row r="29" spans="4:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D29" s="98" t="s">
+      <c r="D29" s="88" t="s">
+        <v>145</v>
+      </c>
+      <c r="E29" s="89"/>
+      <c r="F29" s="89"/>
+      <c r="G29" s="89" t="s">
+        <v>149</v>
+      </c>
+      <c r="H29" s="89"/>
+      <c r="I29" s="89"/>
+      <c r="J29" s="95" t="s">
+        <v>146</v>
+      </c>
+      <c r="K29" s="96"/>
+      <c r="L29" s="97"/>
+    </row>
+    <row r="30" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D30" s="98" t="s">
         <v>147</v>
       </c>
-      <c r="E29" s="99"/>
-      <c r="F29" s="99"/>
-      <c r="G29" s="99" t="s">
-        <v>151</v>
-      </c>
-      <c r="H29" s="99"/>
-      <c r="I29" s="99"/>
-      <c r="J29" s="103" t="s">
-        <v>148</v>
-      </c>
-      <c r="K29" s="104"/>
-      <c r="L29" s="105"/>
-    </row>
-    <row r="30" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D30" s="106" t="s">
-        <v>149</v>
-      </c>
-      <c r="E30" s="85"/>
-      <c r="F30" s="85"/>
-      <c r="G30" s="85">
+      <c r="E30" s="94"/>
+      <c r="F30" s="94"/>
+      <c r="G30" s="94">
         <v>2.121</v>
       </c>
-      <c r="H30" s="85"/>
-      <c r="I30" s="85"/>
-      <c r="J30" s="85">
+      <c r="H30" s="94"/>
+      <c r="I30" s="94"/>
+      <c r="J30" s="94">
         <f>G30*220*0.97</f>
         <v>452.62139999999999</v>
       </c>
-      <c r="K30" s="85"/>
-      <c r="L30" s="86"/>
+      <c r="K30" s="94"/>
+      <c r="L30" s="108"/>
     </row>
     <row r="31" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D31" s="100"/>
-      <c r="E31" s="87"/>
-      <c r="F31" s="87"/>
-      <c r="G31" s="87"/>
-      <c r="H31" s="87"/>
-      <c r="I31" s="87"/>
-      <c r="J31" s="87"/>
-      <c r="K31" s="87"/>
-      <c r="L31" s="88"/>
+      <c r="D31" s="90"/>
+      <c r="E31" s="91"/>
+      <c r="F31" s="91"/>
+      <c r="G31" s="91"/>
+      <c r="H31" s="91"/>
+      <c r="I31" s="91"/>
+      <c r="J31" s="91"/>
+      <c r="K31" s="91"/>
+      <c r="L31" s="109"/>
     </row>
     <row r="32" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D32" s="100"/>
-      <c r="E32" s="87"/>
-      <c r="F32" s="87"/>
-      <c r="G32" s="87"/>
-      <c r="H32" s="87"/>
-      <c r="I32" s="87"/>
-      <c r="J32" s="87"/>
-      <c r="K32" s="87"/>
-      <c r="L32" s="88"/>
+      <c r="D32" s="90"/>
+      <c r="E32" s="91"/>
+      <c r="F32" s="91"/>
+      <c r="G32" s="91"/>
+      <c r="H32" s="91"/>
+      <c r="I32" s="91"/>
+      <c r="J32" s="91"/>
+      <c r="K32" s="91"/>
+      <c r="L32" s="109"/>
     </row>
     <row r="33" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D33" s="100" t="s">
-        <v>150</v>
-      </c>
-      <c r="E33" s="87"/>
-      <c r="F33" s="87"/>
-      <c r="G33" s="87">
+      <c r="D33" s="90" t="s">
+        <v>148</v>
+      </c>
+      <c r="E33" s="91"/>
+      <c r="F33" s="91"/>
+      <c r="G33" s="91">
         <v>2.1259999999999999</v>
       </c>
-      <c r="H33" s="87"/>
-      <c r="I33" s="87"/>
-      <c r="J33" s="76">
+      <c r="H33" s="91"/>
+      <c r="I33" s="91"/>
+      <c r="J33" s="99">
         <f t="shared" ref="J33" si="7">G33*230*0.97</f>
         <v>474.31059999999997</v>
       </c>
-      <c r="K33" s="77"/>
-      <c r="L33" s="78"/>
+      <c r="K33" s="100"/>
+      <c r="L33" s="101"/>
     </row>
     <row r="34" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D34" s="100"/>
-      <c r="E34" s="87"/>
-      <c r="F34" s="87"/>
-      <c r="G34" s="87"/>
-      <c r="H34" s="87"/>
-      <c r="I34" s="87"/>
-      <c r="J34" s="79"/>
-      <c r="K34" s="80"/>
-      <c r="L34" s="81"/>
+      <c r="D34" s="90"/>
+      <c r="E34" s="91"/>
+      <c r="F34" s="91"/>
+      <c r="G34" s="91"/>
+      <c r="H34" s="91"/>
+      <c r="I34" s="91"/>
+      <c r="J34" s="102"/>
+      <c r="K34" s="103"/>
+      <c r="L34" s="104"/>
     </row>
     <row r="35" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D35" s="100"/>
-      <c r="E35" s="87"/>
-      <c r="F35" s="87"/>
-      <c r="G35" s="87"/>
-      <c r="H35" s="87"/>
-      <c r="I35" s="87"/>
-      <c r="J35" s="89"/>
-      <c r="K35" s="90"/>
-      <c r="L35" s="91"/>
+      <c r="D35" s="90"/>
+      <c r="E35" s="91"/>
+      <c r="F35" s="91"/>
+      <c r="G35" s="91"/>
+      <c r="H35" s="91"/>
+      <c r="I35" s="91"/>
+      <c r="J35" s="110"/>
+      <c r="K35" s="111"/>
+      <c r="L35" s="112"/>
     </row>
     <row r="36" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D36" s="100" t="s">
-        <v>152</v>
-      </c>
-      <c r="E36" s="87"/>
-      <c r="F36" s="87"/>
-      <c r="G36" s="87">
+      <c r="D36" s="90" t="s">
+        <v>150</v>
+      </c>
+      <c r="E36" s="91"/>
+      <c r="F36" s="91"/>
+      <c r="G36" s="91">
         <v>2.2250000000000001</v>
       </c>
-      <c r="H36" s="87"/>
-      <c r="I36" s="87"/>
-      <c r="J36" s="76">
+      <c r="H36" s="91"/>
+      <c r="I36" s="91"/>
+      <c r="J36" s="99">
         <f t="shared" ref="J36" si="8">G36*230*0.97</f>
         <v>496.39749999999998</v>
       </c>
-      <c r="K36" s="77"/>
-      <c r="L36" s="78"/>
+      <c r="K36" s="100"/>
+      <c r="L36" s="101"/>
     </row>
     <row r="37" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D37" s="100"/>
-      <c r="E37" s="87"/>
-      <c r="F37" s="87"/>
-      <c r="G37" s="87"/>
-      <c r="H37" s="87"/>
-      <c r="I37" s="87"/>
-      <c r="J37" s="79"/>
-      <c r="K37" s="80"/>
-      <c r="L37" s="81"/>
+      <c r="D37" s="90"/>
+      <c r="E37" s="91"/>
+      <c r="F37" s="91"/>
+      <c r="G37" s="91"/>
+      <c r="H37" s="91"/>
+      <c r="I37" s="91"/>
+      <c r="J37" s="102"/>
+      <c r="K37" s="103"/>
+      <c r="L37" s="104"/>
     </row>
     <row r="38" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D38" s="100"/>
-      <c r="E38" s="87"/>
-      <c r="F38" s="87"/>
-      <c r="G38" s="87"/>
-      <c r="H38" s="87"/>
-      <c r="I38" s="87"/>
-      <c r="J38" s="89"/>
-      <c r="K38" s="90"/>
-      <c r="L38" s="91"/>
+      <c r="D38" s="90"/>
+      <c r="E38" s="91"/>
+      <c r="F38" s="91"/>
+      <c r="G38" s="91"/>
+      <c r="H38" s="91"/>
+      <c r="I38" s="91"/>
+      <c r="J38" s="110"/>
+      <c r="K38" s="111"/>
+      <c r="L38" s="112"/>
     </row>
     <row r="39" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D39" s="100" t="s">
-        <v>153</v>
-      </c>
-      <c r="E39" s="87"/>
-      <c r="F39" s="87"/>
-      <c r="G39" s="87">
+      <c r="D39" s="90" t="s">
+        <v>151</v>
+      </c>
+      <c r="E39" s="91"/>
+      <c r="F39" s="91"/>
+      <c r="G39" s="91">
         <v>2.242</v>
       </c>
-      <c r="H39" s="87"/>
-      <c r="I39" s="87"/>
-      <c r="J39" s="76">
+      <c r="H39" s="91"/>
+      <c r="I39" s="91"/>
+      <c r="J39" s="99">
         <f t="shared" ref="J39" si="9">G39*230*0.97</f>
         <v>500.19019999999995</v>
       </c>
-      <c r="K39" s="77"/>
-      <c r="L39" s="78"/>
+      <c r="K39" s="100"/>
+      <c r="L39" s="101"/>
     </row>
     <row r="40" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D40" s="100"/>
-      <c r="E40" s="87"/>
-      <c r="F40" s="87"/>
-      <c r="G40" s="87"/>
-      <c r="H40" s="87"/>
-      <c r="I40" s="87"/>
-      <c r="J40" s="79"/>
-      <c r="K40" s="80"/>
-      <c r="L40" s="81"/>
+      <c r="D40" s="90"/>
+      <c r="E40" s="91"/>
+      <c r="F40" s="91"/>
+      <c r="G40" s="91"/>
+      <c r="H40" s="91"/>
+      <c r="I40" s="91"/>
+      <c r="J40" s="102"/>
+      <c r="K40" s="103"/>
+      <c r="L40" s="104"/>
     </row>
     <row r="41" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D41" s="100"/>
-      <c r="E41" s="87"/>
-      <c r="F41" s="87"/>
-      <c r="G41" s="87"/>
-      <c r="H41" s="87"/>
-      <c r="I41" s="87"/>
-      <c r="J41" s="89"/>
-      <c r="K41" s="90"/>
-      <c r="L41" s="91"/>
+      <c r="D41" s="90"/>
+      <c r="E41" s="91"/>
+      <c r="F41" s="91"/>
+      <c r="G41" s="91"/>
+      <c r="H41" s="91"/>
+      <c r="I41" s="91"/>
+      <c r="J41" s="110"/>
+      <c r="K41" s="111"/>
+      <c r="L41" s="112"/>
     </row>
     <row r="42" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D42" s="100" t="s">
-        <v>154</v>
-      </c>
-      <c r="E42" s="87"/>
-      <c r="F42" s="87"/>
-      <c r="G42" s="87">
+      <c r="D42" s="90" t="s">
+        <v>152</v>
+      </c>
+      <c r="E42" s="91"/>
+      <c r="F42" s="91"/>
+      <c r="G42" s="91">
         <v>2.3029999999999999</v>
       </c>
-      <c r="H42" s="87"/>
-      <c r="I42" s="87"/>
-      <c r="J42" s="76">
+      <c r="H42" s="91"/>
+      <c r="I42" s="91"/>
+      <c r="J42" s="99">
         <f t="shared" ref="J42" si="10">G42*230*0.97</f>
         <v>513.7992999999999</v>
       </c>
-      <c r="K42" s="77"/>
-      <c r="L42" s="78"/>
+      <c r="K42" s="100"/>
+      <c r="L42" s="101"/>
     </row>
     <row r="43" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D43" s="100"/>
-      <c r="E43" s="87"/>
-      <c r="F43" s="87"/>
-      <c r="G43" s="87"/>
-      <c r="H43" s="87"/>
-      <c r="I43" s="87"/>
-      <c r="J43" s="79"/>
-      <c r="K43" s="80"/>
-      <c r="L43" s="81"/>
+      <c r="D43" s="90"/>
+      <c r="E43" s="91"/>
+      <c r="F43" s="91"/>
+      <c r="G43" s="91"/>
+      <c r="H43" s="91"/>
+      <c r="I43" s="91"/>
+      <c r="J43" s="102"/>
+      <c r="K43" s="103"/>
+      <c r="L43" s="104"/>
     </row>
     <row r="44" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D44" s="101"/>
-      <c r="E44" s="102"/>
-      <c r="F44" s="102"/>
-      <c r="G44" s="102"/>
-      <c r="H44" s="102"/>
-      <c r="I44" s="102"/>
-      <c r="J44" s="82"/>
-      <c r="K44" s="83"/>
-      <c r="L44" s="84"/>
+      <c r="D44" s="92"/>
+      <c r="E44" s="93"/>
+      <c r="F44" s="93"/>
+      <c r="G44" s="93"/>
+      <c r="H44" s="93"/>
+      <c r="I44" s="93"/>
+      <c r="J44" s="105"/>
+      <c r="K44" s="106"/>
+      <c r="L44" s="107"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="J42:L44"/>
+    <mergeCell ref="J30:L32"/>
+    <mergeCell ref="J33:L35"/>
+    <mergeCell ref="J36:L38"/>
+    <mergeCell ref="J39:L41"/>
     <mergeCell ref="M4:U4"/>
     <mergeCell ref="D4:K4"/>
     <mergeCell ref="D29:F29"/>
@@ -6835,11 +6852,6 @@
     <mergeCell ref="D33:F35"/>
     <mergeCell ref="D36:F38"/>
     <mergeCell ref="G29:I29"/>
-    <mergeCell ref="J42:L44"/>
-    <mergeCell ref="J30:L32"/>
-    <mergeCell ref="J33:L35"/>
-    <mergeCell ref="J36:L38"/>
-    <mergeCell ref="J39:L41"/>
   </mergeCells>
   <conditionalFormatting sqref="K6:K26">
     <cfRule type="top10" dxfId="3" priority="4" rank="3"/>

</xml_diff>